<commit_message>
merge of nimish and anna branch
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="Alternatives" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="158">
   <si>
     <t>Course</t>
   </si>
@@ -319,6 +320,12 @@
     <t>Wilson, Marcella</t>
   </si>
   <si>
+    <t>CMSC 478</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
     <t>CMSC 483/691</t>
   </si>
   <si>
@@ -328,127 +335,160 @@
     <t>Simon, Tyler</t>
   </si>
   <si>
+    <t>CMSC 611</t>
+  </si>
+  <si>
+    <t>Interdisciplinary Life S 237</t>
+  </si>
+  <si>
+    <t>tt1130</t>
+  </si>
+  <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
+    <t>Kalpakis, Kostas</t>
+  </si>
+  <si>
+    <t>tt10</t>
+  </si>
+  <si>
+    <t>Chang, Richard</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>tt230</t>
+  </si>
+  <si>
+    <t>CMSC 411ce</t>
+  </si>
+  <si>
+    <t>Perkins, Dmitri</t>
+  </si>
+  <si>
+    <t>CMSC 479/679</t>
+  </si>
+  <si>
+    <t>Introduction to Robotics</t>
+  </si>
+  <si>
+    <t>Matuszek, Cynthia</t>
+  </si>
+  <si>
+    <t>CMSC 678</t>
+  </si>
+  <si>
+    <t>Oates, Tim</t>
+  </si>
+  <si>
+    <t>tt4</t>
+  </si>
+  <si>
+    <t>CMSC 426</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>Finin, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 481</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>Spec Topic: Computer Vision</t>
+  </si>
+  <si>
+    <t>Chapman, David</t>
+  </si>
+  <si>
+    <t>Liu, Chenchen</t>
+  </si>
+  <si>
+    <t>tt710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spec Topic: Quantum Security </t>
+  </si>
+  <si>
+    <t>CMSC 487/687</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Zieglar, Edward</t>
+  </si>
+  <si>
+    <t>tt1</t>
+  </si>
+  <si>
+    <t>CMSC 493</t>
+  </si>
+  <si>
+    <t>Games Capstone</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>CMSC 621</t>
+  </si>
+  <si>
     <t>CMSC 682</t>
   </si>
   <si>
     <t>Network Technologies</t>
   </si>
   <si>
-    <t>Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>tt1130</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>CMSC 478</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>tt10</t>
-  </si>
-  <si>
-    <t>Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>tt230</t>
-  </si>
-  <si>
-    <t>CMSC 411ce</t>
-  </si>
-  <si>
-    <t>Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 479/679</t>
-  </si>
-  <si>
-    <t>Introduction to Robotics</t>
-  </si>
-  <si>
-    <t>Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 678</t>
-  </si>
-  <si>
-    <t>Oates, Tim</t>
-  </si>
-  <si>
-    <t>tt4</t>
-  </si>
-  <si>
-    <t>CMSC 426</t>
-  </si>
-  <si>
-    <t>Computer Security</t>
-  </si>
-  <si>
-    <t>Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 481</t>
-  </si>
-  <si>
-    <t>Computer Networks</t>
-  </si>
-  <si>
-    <t>Spec Topic: Computer Vision</t>
-  </si>
-  <si>
-    <t>Chapman, David</t>
-  </si>
-  <si>
-    <t>CMSC 611</t>
-  </si>
-  <si>
-    <t>Liu, Chenchen</t>
-  </si>
-  <si>
-    <t>tt710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spec Topic: Quantum Security </t>
-  </si>
-  <si>
-    <t>CMSC 487/687</t>
-  </si>
-  <si>
-    <t>Network Security</t>
-  </si>
-  <si>
-    <t>Zieglar, Edward</t>
-  </si>
-  <si>
-    <t>tt1</t>
-  </si>
-  <si>
-    <t>CMSC 493</t>
-  </si>
-  <si>
-    <t>Games Capstone</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>CMSC 621</t>
+    <t>unscheduled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spec Topic: Internet of Things </t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>alt1</t>
+  </si>
+  <si>
+    <t>alt2</t>
+  </si>
+  <si>
+    <t>alt3</t>
+  </si>
+  <si>
+    <t>CMSC 682Network Technologies2Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>{'mw530': Interdisciplinary Life S 237}</t>
+  </si>
+  <si>
+    <t>{'mw530': Public Policy 105}</t>
+  </si>
+  <si>
+    <t>{'mw230': Sherman Hall 014}</t>
+  </si>
+  <si>
+    <t>CMSC 684Wireless Sensor Networks2Staff</t>
+  </si>
+  <si>
+    <t>CMSC 491/691Spec Topic: Internet of Things 1Staff</t>
   </si>
 </sst>
 </file>
@@ -780,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -849,7 +889,7 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -875,7 +915,7 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -901,7 +941,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1060,7 +1100,7 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -1294,7 +1334,7 @@
         <v>16</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1771,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
@@ -1817,25 +1857,25 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F40">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G40" t="s">
         <v>99</v>
       </c>
       <c r="H40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I40" t="s">
         <v>14</v>
@@ -1843,25 +1883,25 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="F41">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G41" t="s">
         <v>99</v>
       </c>
       <c r="H41" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I41" t="s">
         <v>14</v>
@@ -1869,25 +1909,25 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
       </c>
       <c r="F42">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G42" t="s">
         <v>99</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I42" t="s">
         <v>14</v>
@@ -1895,13 +1935,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
         <v>21</v>
@@ -1913,7 +1953,7 @@
         <v>99</v>
       </c>
       <c r="H43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I43" t="s">
         <v>14</v>
@@ -1921,25 +1961,25 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
         <v>21</v>
       </c>
       <c r="F44">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G44" t="s">
         <v>99</v>
       </c>
       <c r="H44" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="I44" t="s">
         <v>14</v>
@@ -1947,19 +1987,19 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="F45">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G45" t="s">
         <v>99</v>
@@ -1973,19 +2013,19 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="F46">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
         <v>99</v>
@@ -1999,25 +2039,25 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="F47">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H47" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="I47" t="s">
         <v>14</v>
@@ -2025,25 +2065,25 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="F48">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G48" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H48" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I48" t="s">
         <v>14</v>
@@ -2051,25 +2091,25 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="F49">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G49" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H49" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="I49" t="s">
         <v>14</v>
@@ -2077,25 +2117,25 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" t="s">
         <v>21</v>
       </c>
       <c r="F50">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G50" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" t="s">
         <v>107</v>
-      </c>
-      <c r="H50" t="s">
-        <v>22</v>
       </c>
       <c r="I50" t="s">
         <v>14</v>
@@ -2103,25 +2143,25 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="F51">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G51" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H51" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I51" t="s">
         <v>14</v>
@@ -2129,25 +2169,25 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="F52">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H52" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I52" t="s">
         <v>14</v>
@@ -2155,25 +2195,25 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F53">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H53" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I53" t="s">
         <v>14</v>
@@ -2181,25 +2221,25 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>40</v>
+      </c>
+      <c r="G54" t="s">
         <v>108</v>
       </c>
-      <c r="F54">
-        <v>40</v>
-      </c>
-      <c r="G54" t="s">
-        <v>112</v>
-      </c>
       <c r="H54" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I54" t="s">
         <v>14</v>
@@ -2207,25 +2247,25 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="F55">
         <v>40</v>
       </c>
       <c r="G55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H55" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I55" t="s">
         <v>14</v>
@@ -2233,25 +2273,25 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="F56">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G56" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H56" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I56" t="s">
         <v>14</v>
@@ -2259,25 +2299,25 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="F57">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H57" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I57" t="s">
         <v>14</v>
@@ -2285,25 +2325,25 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="F58">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G58" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H58" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="I58" t="s">
         <v>14</v>
@@ -2311,25 +2351,25 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="F59">
         <v>40</v>
       </c>
       <c r="G59" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H59" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="I59" t="s">
         <v>14</v>
@@ -2337,25 +2377,25 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="F60">
         <v>40</v>
       </c>
       <c r="G60" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H60" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I60" t="s">
         <v>14</v>
@@ -2363,25 +2403,25 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F61">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H61" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I61" t="s">
         <v>14</v>
@@ -2389,25 +2429,25 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E62" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="F62">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H62" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I62" t="s">
         <v>14</v>
@@ -2415,25 +2455,25 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="F63">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H63" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I63" t="s">
         <v>14</v>
@@ -2441,25 +2481,25 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F64">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G64" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H64" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I64" t="s">
         <v>14</v>
@@ -2467,25 +2507,25 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="F65">
         <v>40</v>
       </c>
       <c r="G65" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H65" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I65" t="s">
         <v>14</v>
@@ -2493,25 +2533,25 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F66">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G66" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H66" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I66" t="s">
         <v>14</v>
@@ -2519,25 +2559,25 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="D67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="F67">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H67" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I67" t="s">
         <v>14</v>
@@ -2545,25 +2585,25 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="F68">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H68" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I68" t="s">
         <v>14</v>
@@ -2571,25 +2611,25 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="F69">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H69" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I69" t="s">
         <v>14</v>
@@ -2597,28 +2637,25 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
-      </c>
-      <c r="C70" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E70" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="F70">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H70" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I70" t="s">
         <v>14</v>
@@ -2626,25 +2663,25 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="F71">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H71" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="I71" t="s">
         <v>14</v>
@@ -2652,25 +2689,25 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="F72">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G72" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H72" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I72" t="s">
         <v>14</v>
@@ -2678,25 +2715,25 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="D73">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="F73">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G73" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H73" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="I73" t="s">
         <v>14</v>
@@ -2704,25 +2741,28 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>131</v>
+      </c>
+      <c r="C74" t="s">
+        <v>77</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="F74">
         <v>50</v>
       </c>
       <c r="G74" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H74" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I74" t="s">
         <v>14</v>
@@ -2730,25 +2770,25 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F75">
         <v>50</v>
       </c>
       <c r="G75" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H75" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I75" t="s">
         <v>14</v>
@@ -2756,22 +2796,22 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="F76">
         <v>40</v>
       </c>
       <c r="G76" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H76" t="s">
         <v>43</v>
@@ -2782,25 +2822,25 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B77" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E77" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F77">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H77" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="I77" t="s">
         <v>14</v>
@@ -2808,25 +2848,25 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="F78">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G78" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H78" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I78" t="s">
         <v>14</v>
@@ -2834,25 +2874,25 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="F79">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G79" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H79" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="I79" t="s">
         <v>14</v>
@@ -2860,25 +2900,25 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="F80">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H80" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I80" t="s">
         <v>14</v>
@@ -2886,28 +2926,2544 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
+        <v>47</v>
+      </c>
+      <c r="B81" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s">
+        <v>100</v>
+      </c>
+      <c r="F81">
+        <v>40</v>
+      </c>
+      <c r="G81" t="s">
+        <v>139</v>
+      </c>
+      <c r="H81" t="s">
+        <v>18</v>
+      </c>
+      <c r="I81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" t="s">
+        <v>126</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82">
+        <v>40</v>
+      </c>
+      <c r="G82" t="s">
+        <v>139</v>
+      </c>
+      <c r="H82" t="s">
+        <v>22</v>
+      </c>
+      <c r="I82" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" t="s">
+        <v>36</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>112</v>
+      </c>
+      <c r="F83">
+        <v>40</v>
+      </c>
+      <c r="G83" t="s">
+        <v>139</v>
+      </c>
+      <c r="H83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>142</v>
+      </c>
+      <c r="F84">
+        <v>50</v>
+      </c>
+      <c r="G84" t="s">
+        <v>139</v>
+      </c>
+      <c r="H84" t="s">
+        <v>26</v>
+      </c>
+      <c r="I84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>143</v>
+      </c>
+      <c r="B85" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85">
+        <v>50</v>
+      </c>
+      <c r="G85" t="s">
+        <v>139</v>
+      </c>
+      <c r="H85" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86">
+        <v>40</v>
+      </c>
+      <c r="G86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" t="s">
+        <v>43</v>
+      </c>
+      <c r="I86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87">
+        <v>100</v>
+      </c>
+      <c r="G87" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B88" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88" t="s">
+        <v>17</v>
+      </c>
+      <c r="F88">
+        <v>40</v>
+      </c>
+      <c r="G88" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s">
+        <v>18</v>
+      </c>
+      <c r="I88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89">
+        <v>40</v>
+      </c>
+      <c r="G89" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s">
+        <v>22</v>
+      </c>
+      <c r="I89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90">
+        <v>7</v>
+      </c>
+      <c r="E90" t="s">
+        <v>21</v>
+      </c>
+      <c r="F90">
+        <v>40</v>
+      </c>
+      <c r="G90" t="s">
+        <v>12</v>
+      </c>
+      <c r="H90" t="s">
+        <v>23</v>
+      </c>
+      <c r="I90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" t="s">
+        <v>25</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91">
+        <v>40</v>
+      </c>
+      <c r="G91" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
+        <v>27</v>
+      </c>
+      <c r="B92" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92">
+        <v>50</v>
+      </c>
+      <c r="G92" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" t="s">
+        <v>29</v>
+      </c>
+      <c r="I92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>33</v>
+      </c>
+      <c r="F93">
+        <v>50</v>
+      </c>
+      <c r="G93" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" t="s">
+        <v>34</v>
+      </c>
+      <c r="I93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>37</v>
+      </c>
+      <c r="F94">
+        <v>50</v>
+      </c>
+      <c r="G94" t="s">
+        <v>38</v>
+      </c>
+      <c r="H94" t="s">
+        <v>39</v>
+      </c>
+      <c r="I94" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" t="s">
+        <v>40</v>
+      </c>
+      <c r="B95" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95">
+        <v>60</v>
+      </c>
+      <c r="G95" t="s">
+        <v>42</v>
+      </c>
+      <c r="H95" t="s">
+        <v>39</v>
+      </c>
+      <c r="I95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96">
+        <v>7</v>
+      </c>
+      <c r="E96" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96">
+        <v>40</v>
+      </c>
+      <c r="G96" t="s">
+        <v>42</v>
+      </c>
+      <c r="H96" t="s">
+        <v>43</v>
+      </c>
+      <c r="I96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>44</v>
+      </c>
+      <c r="B97" t="s">
+        <v>45</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>46</v>
+      </c>
+      <c r="F97">
+        <v>40</v>
+      </c>
+      <c r="G97" t="s">
+        <v>42</v>
+      </c>
+      <c r="H97" t="s">
+        <v>18</v>
+      </c>
+      <c r="I97" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>47</v>
+      </c>
+      <c r="B98" t="s">
+        <v>48</v>
+      </c>
+      <c r="D98">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98">
+        <v>40</v>
+      </c>
+      <c r="G98" t="s">
+        <v>42</v>
+      </c>
+      <c r="H98" t="s">
+        <v>22</v>
+      </c>
+      <c r="I98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" t="s">
+        <v>51</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s">
+        <v>52</v>
+      </c>
+      <c r="F99">
+        <v>40</v>
+      </c>
+      <c r="G99" t="s">
+        <v>42</v>
+      </c>
+      <c r="H99" t="s">
+        <v>23</v>
+      </c>
+      <c r="I99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" t="s">
+        <v>54</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>55</v>
+      </c>
+      <c r="F100">
+        <v>30</v>
+      </c>
+      <c r="G100" t="s">
+        <v>42</v>
+      </c>
+      <c r="H100" t="s">
+        <v>56</v>
+      </c>
+      <c r="I100" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>57</v>
+      </c>
+      <c r="B101" t="s">
+        <v>58</v>
+      </c>
+      <c r="D101">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>21</v>
+      </c>
+      <c r="F101">
+        <v>40</v>
+      </c>
+      <c r="G101" t="s">
+        <v>42</v>
+      </c>
+      <c r="H101" t="s">
+        <v>26</v>
+      </c>
+      <c r="I101" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102">
+        <v>40</v>
+      </c>
+      <c r="G102" t="s">
+        <v>42</v>
+      </c>
+      <c r="H102" t="s">
+        <v>29</v>
+      </c>
+      <c r="I102" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>62</v>
+      </c>
+      <c r="B103" t="s">
+        <v>41</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>17</v>
+      </c>
+      <c r="F103">
+        <v>120</v>
+      </c>
+      <c r="G103" t="s">
+        <v>63</v>
+      </c>
+      <c r="H103" t="s">
+        <v>64</v>
+      </c>
+      <c r="I103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>9</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>5</v>
+      </c>
+      <c r="E104" t="s">
+        <v>65</v>
+      </c>
+      <c r="F104">
+        <v>100</v>
+      </c>
+      <c r="G104" t="s">
+        <v>63</v>
+      </c>
+      <c r="H104" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>15</v>
+      </c>
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105">
+        <v>6</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105">
+        <v>40</v>
+      </c>
+      <c r="G105" t="s">
+        <v>63</v>
+      </c>
+      <c r="H105" t="s">
+        <v>43</v>
+      </c>
+      <c r="I105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106" t="s">
+        <v>45</v>
+      </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+      <c r="E106" t="s">
+        <v>66</v>
+      </c>
+      <c r="F106">
+        <v>40</v>
+      </c>
+      <c r="G106" t="s">
+        <v>63</v>
+      </c>
+      <c r="H106" t="s">
+        <v>18</v>
+      </c>
+      <c r="I106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>67</v>
+      </c>
+      <c r="B107" t="s">
+        <v>68</v>
+      </c>
+      <c r="D107">
+        <v>3</v>
+      </c>
+      <c r="E107" t="s">
+        <v>69</v>
+      </c>
+      <c r="F107">
+        <v>40</v>
+      </c>
+      <c r="G107" t="s">
+        <v>63</v>
+      </c>
+      <c r="H107" t="s">
+        <v>22</v>
+      </c>
+      <c r="I107" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>47</v>
+      </c>
+      <c r="B108" t="s">
+        <v>48</v>
+      </c>
+      <c r="D108">
+        <v>4</v>
+      </c>
+      <c r="E108" t="s">
+        <v>70</v>
+      </c>
+      <c r="F108">
+        <v>40</v>
+      </c>
+      <c r="G108" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108" t="s">
+        <v>23</v>
+      </c>
+      <c r="I108" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" t="s">
+        <v>51</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>46</v>
+      </c>
+      <c r="F109">
+        <v>40</v>
+      </c>
+      <c r="G109" t="s">
+        <v>63</v>
+      </c>
+      <c r="H109" t="s">
+        <v>26</v>
+      </c>
+      <c r="I109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>71</v>
+      </c>
+      <c r="B110" t="s">
+        <v>72</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>52</v>
+      </c>
+      <c r="F110">
+        <v>50</v>
+      </c>
+      <c r="G110" t="s">
+        <v>63</v>
+      </c>
+      <c r="H110" t="s">
+        <v>29</v>
+      </c>
+      <c r="I110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>53</v>
+      </c>
+      <c r="B111" t="s">
+        <v>54</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>55</v>
+      </c>
+      <c r="F111">
+        <v>30</v>
+      </c>
+      <c r="G111" t="s">
+        <v>63</v>
+      </c>
+      <c r="H111" t="s">
+        <v>56</v>
+      </c>
+      <c r="I111" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>73</v>
+      </c>
+      <c r="B112" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>75</v>
+      </c>
+      <c r="F112">
+        <v>50</v>
+      </c>
+      <c r="G112" t="s">
+        <v>63</v>
+      </c>
+      <c r="H112" t="s">
+        <v>34</v>
+      </c>
+      <c r="I112" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" t="s">
+        <v>76</v>
+      </c>
+      <c r="C113" t="s">
+        <v>77</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" t="s">
+        <v>78</v>
+      </c>
+      <c r="F113">
+        <v>50</v>
+      </c>
+      <c r="G113" t="s">
+        <v>63</v>
+      </c>
+      <c r="H113" t="s">
+        <v>39</v>
+      </c>
+      <c r="I113" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>62</v>
+      </c>
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114" t="s">
+        <v>17</v>
+      </c>
+      <c r="F114">
+        <v>100</v>
+      </c>
+      <c r="G114" t="s">
+        <v>79</v>
+      </c>
+      <c r="H114" t="s">
+        <v>13</v>
+      </c>
+      <c r="I114" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>47</v>
+      </c>
+      <c r="B115" t="s">
+        <v>48</v>
+      </c>
+      <c r="D115">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>70</v>
+      </c>
+      <c r="F115">
+        <v>40</v>
+      </c>
+      <c r="G115" t="s">
+        <v>79</v>
+      </c>
+      <c r="H115" t="s">
+        <v>43</v>
+      </c>
+      <c r="I115" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>80</v>
+      </c>
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+      <c r="D116">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>82</v>
+      </c>
+      <c r="F116">
+        <v>40</v>
+      </c>
+      <c r="G116" t="s">
+        <v>79</v>
+      </c>
+      <c r="H116" t="s">
+        <v>18</v>
+      </c>
+      <c r="I116" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>27</v>
+      </c>
+      <c r="B117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>83</v>
+      </c>
+      <c r="F117">
+        <v>50</v>
+      </c>
+      <c r="G117" t="s">
+        <v>79</v>
+      </c>
+      <c r="H117" t="s">
+        <v>26</v>
+      </c>
+      <c r="I117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>84</v>
+      </c>
+      <c r="B118" t="s">
+        <v>85</v>
+      </c>
+      <c r="C118" t="s">
+        <v>86</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118" t="s">
+        <v>55</v>
+      </c>
+      <c r="F118">
+        <v>40</v>
+      </c>
+      <c r="G118" t="s">
+        <v>79</v>
+      </c>
+      <c r="H118" t="s">
+        <v>22</v>
+      </c>
+      <c r="I118" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
+        <v>88</v>
+      </c>
+      <c r="C119" t="s">
+        <v>89</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
+        <v>90</v>
+      </c>
+      <c r="F119">
+        <v>50</v>
+      </c>
+      <c r="G119" t="s">
+        <v>79</v>
+      </c>
+      <c r="H119" t="s">
+        <v>29</v>
+      </c>
+      <c r="I119" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>91</v>
+      </c>
+      <c r="B120" t="s">
+        <v>92</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
+        <v>21</v>
+      </c>
+      <c r="F120">
+        <v>30</v>
+      </c>
+      <c r="G120" t="s">
+        <v>93</v>
+      </c>
+      <c r="H120" t="s">
+        <v>56</v>
+      </c>
+      <c r="I120" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>47</v>
+      </c>
+      <c r="B121" t="s">
+        <v>48</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" t="s">
+        <v>94</v>
+      </c>
+      <c r="F121">
+        <v>40</v>
+      </c>
+      <c r="G121" t="s">
+        <v>93</v>
+      </c>
+      <c r="H121" t="s">
+        <v>43</v>
+      </c>
+      <c r="I121" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>95</v>
+      </c>
+      <c r="B122" t="s">
+        <v>36</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122" t="s">
+        <v>94</v>
+      </c>
+      <c r="F122">
+        <v>40</v>
+      </c>
+      <c r="G122" t="s">
+        <v>93</v>
+      </c>
+      <c r="H122" t="s">
+        <v>18</v>
+      </c>
+      <c r="I122" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>19</v>
+      </c>
+      <c r="B123" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123">
+        <v>5</v>
+      </c>
+      <c r="E123" t="s">
+        <v>21</v>
+      </c>
+      <c r="F123">
+        <v>40</v>
+      </c>
+      <c r="G123" t="s">
+        <v>96</v>
+      </c>
+      <c r="H123" t="s">
+        <v>43</v>
+      </c>
+      <c r="I123" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>97</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124" t="s">
+        <v>21</v>
+      </c>
+      <c r="F124">
+        <v>40</v>
+      </c>
+      <c r="G124" t="s">
+        <v>99</v>
+      </c>
+      <c r="H124" t="s">
+        <v>43</v>
+      </c>
+      <c r="I124" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>97</v>
+      </c>
+      <c r="B125" t="s">
+        <v>98</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
+      </c>
+      <c r="E125" t="s">
+        <v>21</v>
+      </c>
+      <c r="F125">
+        <v>40</v>
+      </c>
+      <c r="G125" t="s">
+        <v>99</v>
+      </c>
+      <c r="H125" t="s">
+        <v>18</v>
+      </c>
+      <c r="I125" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>15</v>
+      </c>
+      <c r="B126" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126" t="s">
+        <v>100</v>
+      </c>
+      <c r="F126">
+        <v>80</v>
+      </c>
+      <c r="G126" t="s">
+        <v>99</v>
+      </c>
+      <c r="H126" t="s">
+        <v>13</v>
+      </c>
+      <c r="I126" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>15</v>
+      </c>
+      <c r="B127" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127">
+        <v>2</v>
+      </c>
+      <c r="E127" t="s">
+        <v>21</v>
+      </c>
+      <c r="F127">
+        <v>80</v>
+      </c>
+      <c r="G127" t="s">
+        <v>99</v>
+      </c>
+      <c r="H127" t="s">
+        <v>64</v>
+      </c>
+      <c r="I127" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128" t="s">
+        <v>20</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" t="s">
+        <v>21</v>
+      </c>
+      <c r="F128">
+        <v>40</v>
+      </c>
+      <c r="G128" t="s">
+        <v>99</v>
+      </c>
+      <c r="H128" t="s">
+        <v>22</v>
+      </c>
+      <c r="I128" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" t="s">
+        <v>19</v>
+      </c>
+      <c r="B129" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129">
+        <v>2</v>
+      </c>
+      <c r="E129" t="s">
+        <v>21</v>
+      </c>
+      <c r="F129">
+        <v>40</v>
+      </c>
+      <c r="G129" t="s">
+        <v>99</v>
+      </c>
+      <c r="H129" t="s">
+        <v>23</v>
+      </c>
+      <c r="I129" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
+        <v>19</v>
+      </c>
+      <c r="B130" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130">
+        <v>6</v>
+      </c>
+      <c r="E130" t="s">
+        <v>21</v>
+      </c>
+      <c r="F130">
+        <v>40</v>
+      </c>
+      <c r="G130" t="s">
+        <v>99</v>
+      </c>
+      <c r="H130" t="s">
+        <v>26</v>
+      </c>
+      <c r="I130" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
+        <v>50</v>
+      </c>
+      <c r="B131" t="s">
+        <v>51</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131" t="s">
+        <v>21</v>
+      </c>
+      <c r="F131">
+        <v>40</v>
+      </c>
+      <c r="G131" t="s">
+        <v>99</v>
+      </c>
+      <c r="H131" t="s">
+        <v>29</v>
+      </c>
+      <c r="I131" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>53</v>
+      </c>
+      <c r="B132" t="s">
+        <v>54</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+      <c r="E132" t="s">
+        <v>21</v>
+      </c>
+      <c r="F132">
+        <v>30</v>
+      </c>
+      <c r="G132" t="s">
+        <v>99</v>
+      </c>
+      <c r="H132" t="s">
+        <v>56</v>
+      </c>
+      <c r="I132" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>101</v>
+      </c>
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133" t="s">
+        <v>21</v>
+      </c>
+      <c r="F133">
+        <v>50</v>
+      </c>
+      <c r="G133" t="s">
+        <v>99</v>
+      </c>
+      <c r="H133" t="s">
+        <v>34</v>
+      </c>
+      <c r="I133" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>103</v>
+      </c>
+      <c r="B134" t="s">
+        <v>104</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
+        <v>105</v>
+      </c>
+      <c r="F134">
+        <v>50</v>
+      </c>
+      <c r="G134" t="s">
+        <v>99</v>
+      </c>
+      <c r="H134" t="s">
+        <v>39</v>
+      </c>
+      <c r="I134" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>106</v>
+      </c>
+      <c r="B135" t="s">
+        <v>51</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+      <c r="E135" t="s">
+        <v>21</v>
+      </c>
+      <c r="F135">
+        <v>50</v>
+      </c>
+      <c r="G135" t="s">
+        <v>99</v>
+      </c>
+      <c r="H135" t="s">
+        <v>107</v>
+      </c>
+      <c r="I135" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>62</v>
+      </c>
+      <c r="B136" t="s">
+        <v>41</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="E136" t="s">
+        <v>70</v>
+      </c>
+      <c r="F136">
+        <v>100</v>
+      </c>
+      <c r="G136" t="s">
+        <v>108</v>
+      </c>
+      <c r="H136" t="s">
+        <v>13</v>
+      </c>
+      <c r="I136" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137" t="s">
+        <v>15</v>
+      </c>
+      <c r="B137" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137" t="s">
+        <v>109</v>
+      </c>
+      <c r="F137">
+        <v>40</v>
+      </c>
+      <c r="G137" t="s">
+        <v>108</v>
+      </c>
+      <c r="H137" t="s">
+        <v>43</v>
+      </c>
+      <c r="I137" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" t="s">
+        <v>44</v>
+      </c>
+      <c r="B138" t="s">
+        <v>45</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138" t="s">
+        <v>46</v>
+      </c>
+      <c r="F138">
+        <v>40</v>
+      </c>
+      <c r="G138" t="s">
+        <v>108</v>
+      </c>
+      <c r="H138" t="s">
+        <v>18</v>
+      </c>
+      <c r="I138" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" t="s">
+        <v>24</v>
+      </c>
+      <c r="B139" t="s">
+        <v>25</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139" t="s">
+        <v>21</v>
+      </c>
+      <c r="F139">
+        <v>40</v>
+      </c>
+      <c r="G139" t="s">
+        <v>108</v>
+      </c>
+      <c r="H139" t="s">
+        <v>22</v>
+      </c>
+      <c r="I139" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" t="s">
+        <v>57</v>
+      </c>
+      <c r="B140" t="s">
+        <v>58</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>110</v>
+      </c>
+      <c r="F140">
+        <v>40</v>
+      </c>
+      <c r="G140" t="s">
+        <v>108</v>
+      </c>
+      <c r="H140" t="s">
+        <v>23</v>
+      </c>
+      <c r="I140" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" t="s">
+        <v>101</v>
+      </c>
+      <c r="B141" t="s">
+        <v>102</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="E141" t="s">
+        <v>83</v>
+      </c>
+      <c r="F141">
+        <v>50</v>
+      </c>
+      <c r="G141" t="s">
+        <v>108</v>
+      </c>
+      <c r="H141" t="s">
+        <v>26</v>
+      </c>
+      <c r="I141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" t="s">
+        <v>9</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>65</v>
+      </c>
+      <c r="F142">
+        <v>100</v>
+      </c>
+      <c r="G142" t="s">
+        <v>111</v>
+      </c>
+      <c r="H142" t="s">
+        <v>13</v>
+      </c>
+      <c r="I142" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" t="s">
+        <v>15</v>
+      </c>
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143">
+        <v>4</v>
+      </c>
+      <c r="E143" t="s">
+        <v>109</v>
+      </c>
+      <c r="F143">
+        <v>40</v>
+      </c>
+      <c r="G143" t="s">
+        <v>111</v>
+      </c>
+      <c r="H143" t="s">
+        <v>43</v>
+      </c>
+      <c r="I143" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" t="s">
+        <v>67</v>
+      </c>
+      <c r="B144" t="s">
+        <v>68</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144" t="s">
+        <v>69</v>
+      </c>
+      <c r="F144">
+        <v>40</v>
+      </c>
+      <c r="G144" t="s">
+        <v>111</v>
+      </c>
+      <c r="H144" t="s">
+        <v>18</v>
+      </c>
+      <c r="I144" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" t="s">
+        <v>95</v>
+      </c>
+      <c r="B145" t="s">
+        <v>36</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+      <c r="E145" t="s">
+        <v>112</v>
+      </c>
+      <c r="F145">
+        <v>40</v>
+      </c>
+      <c r="G145" t="s">
+        <v>111</v>
+      </c>
+      <c r="H145" t="s">
+        <v>22</v>
+      </c>
+      <c r="I145" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" t="s">
+        <v>113</v>
+      </c>
+      <c r="B146" t="s">
+        <v>114</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>115</v>
+      </c>
+      <c r="F146">
+        <v>50</v>
+      </c>
+      <c r="G146" t="s">
+        <v>111</v>
+      </c>
+      <c r="H146" t="s">
+        <v>26</v>
+      </c>
+      <c r="I146" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" t="s">
+        <v>9</v>
+      </c>
+      <c r="B147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147">
+        <v>3</v>
+      </c>
+      <c r="E147" t="s">
+        <v>69</v>
+      </c>
+      <c r="F147">
+        <v>100</v>
+      </c>
+      <c r="G147" t="s">
+        <v>116</v>
+      </c>
+      <c r="H147" t="s">
+        <v>13</v>
+      </c>
+      <c r="I147" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="A148" t="s">
+        <v>47</v>
+      </c>
+      <c r="B148" t="s">
+        <v>48</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+      <c r="E148" t="s">
+        <v>100</v>
+      </c>
+      <c r="F148">
+        <v>40</v>
+      </c>
+      <c r="G148" t="s">
+        <v>116</v>
+      </c>
+      <c r="H148" t="s">
+        <v>43</v>
+      </c>
+      <c r="I148" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" t="s">
+        <v>117</v>
+      </c>
+      <c r="B149" t="s">
+        <v>51</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
+        <v>82</v>
+      </c>
+      <c r="F149">
+        <v>40</v>
+      </c>
+      <c r="G149" t="s">
+        <v>116</v>
+      </c>
+      <c r="H149" t="s">
+        <v>18</v>
+      </c>
+      <c r="I149" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" t="s">
+        <v>24</v>
+      </c>
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="D150">
+        <v>2</v>
+      </c>
+      <c r="E150" t="s">
+        <v>118</v>
+      </c>
+      <c r="F150">
+        <v>40</v>
+      </c>
+      <c r="G150" t="s">
+        <v>116</v>
+      </c>
+      <c r="H150" t="s">
+        <v>22</v>
+      </c>
+      <c r="I150" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" t="s">
+        <v>119</v>
+      </c>
+      <c r="B151" t="s">
+        <v>120</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151" t="s">
+        <v>121</v>
+      </c>
+      <c r="F151">
+        <v>50</v>
+      </c>
+      <c r="G151" t="s">
+        <v>116</v>
+      </c>
+      <c r="H151" t="s">
+        <v>26</v>
+      </c>
+      <c r="I151" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" t="s">
+        <v>122</v>
+      </c>
+      <c r="B152" t="s">
+        <v>102</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152" t="s">
+        <v>123</v>
+      </c>
+      <c r="F152">
+        <v>50</v>
+      </c>
+      <c r="G152" t="s">
+        <v>116</v>
+      </c>
+      <c r="H152" t="s">
+        <v>29</v>
+      </c>
+      <c r="I152" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153" t="s">
+        <v>9</v>
+      </c>
+      <c r="B153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153">
+        <v>4</v>
+      </c>
+      <c r="E153" t="s">
+        <v>69</v>
+      </c>
+      <c r="F153">
+        <v>100</v>
+      </c>
+      <c r="G153" t="s">
+        <v>124</v>
+      </c>
+      <c r="H153" t="s">
+        <v>13</v>
+      </c>
+      <c r="I153" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" t="s">
+        <v>44</v>
+      </c>
+      <c r="B154" t="s">
+        <v>45</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+      <c r="E154" t="s">
+        <v>46</v>
+      </c>
+      <c r="F154">
+        <v>40</v>
+      </c>
+      <c r="G154" t="s">
+        <v>124</v>
+      </c>
+      <c r="H154" t="s">
+        <v>43</v>
+      </c>
+      <c r="I154" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" t="s">
+        <v>67</v>
+      </c>
+      <c r="B155" t="s">
+        <v>68</v>
+      </c>
+      <c r="D155">
+        <v>4</v>
+      </c>
+      <c r="E155" t="s">
+        <v>83</v>
+      </c>
+      <c r="F155">
+        <v>40</v>
+      </c>
+      <c r="G155" t="s">
+        <v>124</v>
+      </c>
+      <c r="H155" t="s">
+        <v>18</v>
+      </c>
+      <c r="I155" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" t="s">
+        <v>125</v>
+      </c>
+      <c r="B156" t="s">
+        <v>126</v>
+      </c>
+      <c r="D156">
+        <v>3</v>
+      </c>
+      <c r="E156" t="s">
+        <v>21</v>
+      </c>
+      <c r="F156">
+        <v>40</v>
+      </c>
+      <c r="G156" t="s">
+        <v>124</v>
+      </c>
+      <c r="H156" t="s">
+        <v>22</v>
+      </c>
+      <c r="I156" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" t="s">
+        <v>27</v>
+      </c>
+      <c r="B157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157">
+        <v>2</v>
+      </c>
+      <c r="E157" t="s">
+        <v>127</v>
+      </c>
+      <c r="F157">
+        <v>50</v>
+      </c>
+      <c r="G157" t="s">
+        <v>124</v>
+      </c>
+      <c r="H157" t="s">
+        <v>26</v>
+      </c>
+      <c r="I157" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" t="s">
+        <v>128</v>
+      </c>
+      <c r="B158" t="s">
+        <v>129</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158" t="s">
+        <v>130</v>
+      </c>
+      <c r="F158">
+        <v>50</v>
+      </c>
+      <c r="G158" t="s">
+        <v>124</v>
+      </c>
+      <c r="H158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I158" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" t="s">
+        <v>30</v>
+      </c>
+      <c r="B159" t="s">
+        <v>131</v>
+      </c>
+      <c r="C159" t="s">
+        <v>77</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159" t="s">
+        <v>132</v>
+      </c>
+      <c r="F159">
+        <v>50</v>
+      </c>
+      <c r="G159" t="s">
+        <v>124</v>
+      </c>
+      <c r="H159" t="s">
+        <v>34</v>
+      </c>
+      <c r="I159" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160" t="s">
+        <v>106</v>
+      </c>
+      <c r="B160" t="s">
+        <v>51</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160" t="s">
+        <v>133</v>
+      </c>
+      <c r="F160">
+        <v>50</v>
+      </c>
+      <c r="G160" t="s">
+        <v>124</v>
+      </c>
+      <c r="H160" t="s">
+        <v>39</v>
+      </c>
+      <c r="I160" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
+      <c r="A161" t="s">
+        <v>19</v>
+      </c>
+      <c r="B161" t="s">
+        <v>20</v>
+      </c>
+      <c r="D161">
+        <v>3</v>
+      </c>
+      <c r="E161" t="s">
+        <v>21</v>
+      </c>
+      <c r="F161">
+        <v>40</v>
+      </c>
+      <c r="G161" t="s">
+        <v>134</v>
+      </c>
+      <c r="H161" t="s">
+        <v>43</v>
+      </c>
+      <c r="I161" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" t="s">
+        <v>53</v>
+      </c>
+      <c r="B162" t="s">
+        <v>54</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+      <c r="E162" t="s">
+        <v>21</v>
+      </c>
+      <c r="F162">
+        <v>30</v>
+      </c>
+      <c r="G162" t="s">
+        <v>134</v>
+      </c>
+      <c r="H162" t="s">
+        <v>56</v>
+      </c>
+      <c r="I162" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" t="s">
+        <v>87</v>
+      </c>
+      <c r="B163" t="s">
+        <v>135</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163" t="s">
+        <v>130</v>
+      </c>
+      <c r="F163">
+        <v>50</v>
+      </c>
+      <c r="G163" t="s">
+        <v>134</v>
+      </c>
+      <c r="H163" t="s">
+        <v>26</v>
+      </c>
+      <c r="I163" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" t="s">
+        <v>136</v>
+      </c>
+      <c r="B164" t="s">
+        <v>137</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164" t="s">
+        <v>138</v>
+      </c>
+      <c r="F164">
+        <v>50</v>
+      </c>
+      <c r="G164" t="s">
+        <v>134</v>
+      </c>
+      <c r="H164" t="s">
+        <v>29</v>
+      </c>
+      <c r="I164" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" t="s">
+        <v>67</v>
+      </c>
+      <c r="B165" t="s">
+        <v>68</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165" t="s">
+        <v>83</v>
+      </c>
+      <c r="F165">
+        <v>40</v>
+      </c>
+      <c r="G165" t="s">
+        <v>139</v>
+      </c>
+      <c r="H165" t="s">
+        <v>43</v>
+      </c>
+      <c r="I165" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" t="s">
+        <v>47</v>
+      </c>
+      <c r="B166" t="s">
+        <v>48</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+      <c r="E166" t="s">
+        <v>100</v>
+      </c>
+      <c r="F166">
+        <v>40</v>
+      </c>
+      <c r="G166" t="s">
+        <v>139</v>
+      </c>
+      <c r="H166" t="s">
+        <v>18</v>
+      </c>
+      <c r="I166" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" t="s">
+        <v>125</v>
+      </c>
+      <c r="B167" t="s">
+        <v>126</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167" t="s">
+        <v>21</v>
+      </c>
+      <c r="F167">
+        <v>40</v>
+      </c>
+      <c r="G167" t="s">
+        <v>139</v>
+      </c>
+      <c r="H167" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" t="s">
+        <v>95</v>
+      </c>
+      <c r="B168" t="s">
+        <v>36</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168" t="s">
+        <v>112</v>
+      </c>
+      <c r="F168">
+        <v>40</v>
+      </c>
+      <c r="G168" t="s">
+        <v>139</v>
+      </c>
+      <c r="H168" t="s">
+        <v>23</v>
+      </c>
+      <c r="I168" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" t="s">
+        <v>140</v>
+      </c>
+      <c r="B169" t="s">
+        <v>141</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169" t="s">
+        <v>142</v>
+      </c>
+      <c r="F169">
+        <v>50</v>
+      </c>
+      <c r="G169" t="s">
+        <v>139</v>
+      </c>
+      <c r="H169" t="s">
+        <v>26</v>
+      </c>
+      <c r="I169" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" t="s">
+        <v>143</v>
+      </c>
+      <c r="B170" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170" t="s">
+        <v>110</v>
+      </c>
+      <c r="F170">
+        <v>50</v>
+      </c>
+      <c r="G170" t="s">
+        <v>139</v>
+      </c>
+      <c r="H170" t="s">
+        <v>29</v>
+      </c>
+      <c r="I170" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" t="s">
+        <v>35</v>
+      </c>
+      <c r="B171" t="s">
+        <v>36</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171" t="s">
+        <v>37</v>
+      </c>
+      <c r="F171">
+        <v>50</v>
+      </c>
+      <c r="G171" t="s">
+        <v>38</v>
+      </c>
+      <c r="H171" t="s">
+        <v>39</v>
+      </c>
+      <c r="I171" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" t="s">
         <v>144</v>
       </c>
-      <c r="B81" t="s">
-        <v>25</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="E81" t="s">
-        <v>109</v>
-      </c>
-      <c r="F81">
-        <v>50</v>
-      </c>
-      <c r="G81" t="s">
-        <v>140</v>
-      </c>
-      <c r="H81" t="s">
-        <v>29</v>
-      </c>
-      <c r="I81" t="s">
-        <v>14</v>
+      <c r="B172" t="s">
+        <v>145</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172" t="s">
+        <v>21</v>
+      </c>
+      <c r="F172">
+        <v>50</v>
+      </c>
+      <c r="G172" t="s">
+        <v>99</v>
+      </c>
+      <c r="I172" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" t="s">
+        <v>144</v>
+      </c>
+      <c r="B173" t="s">
+        <v>145</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+      <c r="E173" t="s">
+        <v>130</v>
+      </c>
+      <c r="F173">
+        <v>50</v>
+      </c>
+      <c r="G173" t="s">
+        <v>99</v>
+      </c>
+      <c r="I173" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" t="s">
+        <v>59</v>
+      </c>
+      <c r="B174" t="s">
+        <v>60</v>
+      </c>
+      <c r="D174">
+        <v>2</v>
+      </c>
+      <c r="E174" t="s">
+        <v>21</v>
+      </c>
+      <c r="F174">
+        <v>40</v>
+      </c>
+      <c r="G174" t="s">
+        <v>99</v>
+      </c>
+      <c r="I174" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" t="s">
+        <v>30</v>
+      </c>
+      <c r="B175" t="s">
+        <v>147</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175" t="s">
+        <v>21</v>
+      </c>
+      <c r="F175">
+        <v>50</v>
+      </c>
+      <c r="G175" t="s">
+        <v>99</v>
+      </c>
+      <c r="I175" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed room scheduling from dictionaries to room object in course
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="158">
   <si>
     <t>Course</t>
   </si>
@@ -5321,9 +5321,6 @@
       <c r="F172">
         <v>50</v>
       </c>
-      <c r="G172" t="s">
-        <v>99</v>
-      </c>
       <c r="I172" t="s">
         <v>146</v>
       </c>
@@ -5344,9 +5341,6 @@
       <c r="F173">
         <v>50</v>
       </c>
-      <c r="G173" t="s">
-        <v>99</v>
-      </c>
       <c r="I173" t="s">
         <v>146</v>
       </c>
@@ -5367,9 +5361,6 @@
       <c r="F174">
         <v>40</v>
       </c>
-      <c r="G174" t="s">
-        <v>99</v>
-      </c>
       <c r="I174" t="s">
         <v>146</v>
       </c>
@@ -5389,9 +5380,6 @@
       </c>
       <c r="F175">
         <v>50</v>
-      </c>
-      <c r="G175" t="s">
-        <v>99</v>
       </c>
       <c r="I175" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
fix duplication in output
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="158">
   <si>
     <t>Course</t>
   </si>
@@ -820,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3056,2332 +3056,81 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
         <v>21</v>
       </c>
       <c r="F86">
-        <v>40</v>
-      </c>
-      <c r="G86" t="s">
-        <v>12</v>
-      </c>
-      <c r="H86" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I86" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="D87">
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="F87">
-        <v>100</v>
-      </c>
-      <c r="G87" t="s">
-        <v>12</v>
-      </c>
-      <c r="H87" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="I87" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F88">
         <v>40</v>
       </c>
-      <c r="G88" t="s">
-        <v>12</v>
-      </c>
-      <c r="H88" t="s">
-        <v>18</v>
-      </c>
       <c r="I88" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E89" t="s">
         <v>21</v>
       </c>
       <c r="F89">
-        <v>40</v>
-      </c>
-      <c r="G89" t="s">
-        <v>12</v>
-      </c>
-      <c r="H89" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="I89" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" t="s">
-        <v>19</v>
-      </c>
-      <c r="B90" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90">
-        <v>7</v>
-      </c>
-      <c r="E90" t="s">
-        <v>21</v>
-      </c>
-      <c r="F90">
-        <v>40</v>
-      </c>
-      <c r="G90" t="s">
-        <v>12</v>
-      </c>
-      <c r="H90" t="s">
-        <v>23</v>
-      </c>
-      <c r="I90" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" t="s">
-        <v>24</v>
-      </c>
-      <c r="B91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D91">
-        <v>3</v>
-      </c>
-      <c r="E91" t="s">
-        <v>21</v>
-      </c>
-      <c r="F91">
-        <v>40</v>
-      </c>
-      <c r="G91" t="s">
-        <v>12</v>
-      </c>
-      <c r="H91" t="s">
-        <v>26</v>
-      </c>
-      <c r="I91" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" t="s">
-        <v>27</v>
-      </c>
-      <c r="B92" t="s">
-        <v>28</v>
-      </c>
-      <c r="D92">
-        <v>3</v>
-      </c>
-      <c r="E92" t="s">
-        <v>21</v>
-      </c>
-      <c r="F92">
-        <v>50</v>
-      </c>
-      <c r="G92" t="s">
-        <v>12</v>
-      </c>
-      <c r="H92" t="s">
-        <v>29</v>
-      </c>
-      <c r="I92" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" t="s">
-        <v>30</v>
-      </c>
-      <c r="B93" t="s">
-        <v>31</v>
-      </c>
-      <c r="C93" t="s">
-        <v>32</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
-      </c>
-      <c r="E93" t="s">
-        <v>33</v>
-      </c>
-      <c r="F93">
-        <v>50</v>
-      </c>
-      <c r="G93" t="s">
-        <v>12</v>
-      </c>
-      <c r="H93" t="s">
-        <v>34</v>
-      </c>
-      <c r="I93" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" t="s">
-        <v>35</v>
-      </c>
-      <c r="B94" t="s">
-        <v>36</v>
-      </c>
-      <c r="D94">
-        <v>1</v>
-      </c>
-      <c r="E94" t="s">
-        <v>37</v>
-      </c>
-      <c r="F94">
-        <v>50</v>
-      </c>
-      <c r="G94" t="s">
-        <v>38</v>
-      </c>
-      <c r="H94" t="s">
-        <v>39</v>
-      </c>
-      <c r="I94" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" t="s">
-        <v>40</v>
-      </c>
-      <c r="B95" t="s">
-        <v>41</v>
-      </c>
-      <c r="D95">
-        <v>1</v>
-      </c>
-      <c r="E95" t="s">
-        <v>21</v>
-      </c>
-      <c r="F95">
-        <v>60</v>
-      </c>
-      <c r="G95" t="s">
-        <v>42</v>
-      </c>
-      <c r="H95" t="s">
-        <v>39</v>
-      </c>
-      <c r="I95" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" t="s">
-        <v>15</v>
-      </c>
-      <c r="B96" t="s">
-        <v>16</v>
-      </c>
-      <c r="D96">
-        <v>7</v>
-      </c>
-      <c r="E96" t="s">
-        <v>11</v>
-      </c>
-      <c r="F96">
-        <v>40</v>
-      </c>
-      <c r="G96" t="s">
-        <v>42</v>
-      </c>
-      <c r="H96" t="s">
-        <v>43</v>
-      </c>
-      <c r="I96" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" t="s">
-        <v>44</v>
-      </c>
-      <c r="B97" t="s">
-        <v>45</v>
-      </c>
-      <c r="D97">
-        <v>4</v>
-      </c>
-      <c r="E97" t="s">
-        <v>46</v>
-      </c>
-      <c r="F97">
-        <v>40</v>
-      </c>
-      <c r="G97" t="s">
-        <v>42</v>
-      </c>
-      <c r="H97" t="s">
-        <v>18</v>
-      </c>
-      <c r="I97" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" t="s">
-        <v>47</v>
-      </c>
-      <c r="B98" t="s">
-        <v>48</v>
-      </c>
-      <c r="D98">
-        <v>5</v>
-      </c>
-      <c r="E98" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98">
-        <v>40</v>
-      </c>
-      <c r="G98" t="s">
-        <v>42</v>
-      </c>
-      <c r="H98" t="s">
-        <v>22</v>
-      </c>
-      <c r="I98" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" t="s">
-        <v>50</v>
-      </c>
-      <c r="B99" t="s">
-        <v>51</v>
-      </c>
-      <c r="D99">
-        <v>2</v>
-      </c>
-      <c r="E99" t="s">
-        <v>52</v>
-      </c>
-      <c r="F99">
-        <v>40</v>
-      </c>
-      <c r="G99" t="s">
-        <v>42</v>
-      </c>
-      <c r="H99" t="s">
-        <v>23</v>
-      </c>
-      <c r="I99" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" t="s">
-        <v>53</v>
-      </c>
-      <c r="B100" t="s">
-        <v>54</v>
-      </c>
-      <c r="D100">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s">
-        <v>55</v>
-      </c>
-      <c r="F100">
-        <v>30</v>
-      </c>
-      <c r="G100" t="s">
-        <v>42</v>
-      </c>
-      <c r="H100" t="s">
-        <v>56</v>
-      </c>
-      <c r="I100" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" t="s">
-        <v>57</v>
-      </c>
-      <c r="B101" t="s">
-        <v>58</v>
-      </c>
-      <c r="D101">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s">
-        <v>21</v>
-      </c>
-      <c r="F101">
-        <v>40</v>
-      </c>
-      <c r="G101" t="s">
-        <v>42</v>
-      </c>
-      <c r="H101" t="s">
-        <v>26</v>
-      </c>
-      <c r="I101" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" t="s">
-        <v>59</v>
-      </c>
-      <c r="B102" t="s">
-        <v>60</v>
-      </c>
-      <c r="D102">
-        <v>1</v>
-      </c>
-      <c r="E102" t="s">
-        <v>61</v>
-      </c>
-      <c r="F102">
-        <v>40</v>
-      </c>
-      <c r="G102" t="s">
-        <v>42</v>
-      </c>
-      <c r="H102" t="s">
-        <v>29</v>
-      </c>
-      <c r="I102" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" t="s">
-        <v>62</v>
-      </c>
-      <c r="B103" t="s">
-        <v>41</v>
-      </c>
-      <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="E103" t="s">
-        <v>17</v>
-      </c>
-      <c r="F103">
-        <v>120</v>
-      </c>
-      <c r="G103" t="s">
-        <v>63</v>
-      </c>
-      <c r="H103" t="s">
-        <v>64</v>
-      </c>
-      <c r="I103" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" t="s">
-        <v>9</v>
-      </c>
-      <c r="B104" t="s">
-        <v>10</v>
-      </c>
-      <c r="D104">
-        <v>5</v>
-      </c>
-      <c r="E104" t="s">
-        <v>65</v>
-      </c>
-      <c r="F104">
-        <v>100</v>
-      </c>
-      <c r="G104" t="s">
-        <v>63</v>
-      </c>
-      <c r="H104" t="s">
-        <v>13</v>
-      </c>
-      <c r="I104" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" t="s">
-        <v>15</v>
-      </c>
-      <c r="B105" t="s">
-        <v>16</v>
-      </c>
-      <c r="D105">
-        <v>6</v>
-      </c>
-      <c r="E105" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105">
-        <v>40</v>
-      </c>
-      <c r="G105" t="s">
-        <v>63</v>
-      </c>
-      <c r="H105" t="s">
-        <v>43</v>
-      </c>
-      <c r="I105" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" t="s">
-        <v>44</v>
-      </c>
-      <c r="B106" t="s">
-        <v>45</v>
-      </c>
-      <c r="D106">
-        <v>3</v>
-      </c>
-      <c r="E106" t="s">
-        <v>66</v>
-      </c>
-      <c r="F106">
-        <v>40</v>
-      </c>
-      <c r="G106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H106" t="s">
-        <v>18</v>
-      </c>
-      <c r="I106" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" t="s">
-        <v>67</v>
-      </c>
-      <c r="B107" t="s">
-        <v>68</v>
-      </c>
-      <c r="D107">
-        <v>3</v>
-      </c>
-      <c r="E107" t="s">
-        <v>69</v>
-      </c>
-      <c r="F107">
-        <v>40</v>
-      </c>
-      <c r="G107" t="s">
-        <v>63</v>
-      </c>
-      <c r="H107" t="s">
-        <v>22</v>
-      </c>
-      <c r="I107" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" t="s">
-        <v>47</v>
-      </c>
-      <c r="B108" t="s">
-        <v>48</v>
-      </c>
-      <c r="D108">
-        <v>4</v>
-      </c>
-      <c r="E108" t="s">
-        <v>70</v>
-      </c>
-      <c r="F108">
-        <v>40</v>
-      </c>
-      <c r="G108" t="s">
-        <v>63</v>
-      </c>
-      <c r="H108" t="s">
-        <v>23</v>
-      </c>
-      <c r="I108" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="A109" t="s">
-        <v>50</v>
-      </c>
-      <c r="B109" t="s">
-        <v>51</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
-      </c>
-      <c r="E109" t="s">
-        <v>46</v>
-      </c>
-      <c r="F109">
-        <v>40</v>
-      </c>
-      <c r="G109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H109" t="s">
-        <v>26</v>
-      </c>
-      <c r="I109" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" t="s">
-        <v>71</v>
-      </c>
-      <c r="B110" t="s">
-        <v>72</v>
-      </c>
-      <c r="D110">
-        <v>1</v>
-      </c>
-      <c r="E110" t="s">
-        <v>52</v>
-      </c>
-      <c r="F110">
-        <v>50</v>
-      </c>
-      <c r="G110" t="s">
-        <v>63</v>
-      </c>
-      <c r="H110" t="s">
-        <v>29</v>
-      </c>
-      <c r="I110" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
-      <c r="A111" t="s">
-        <v>53</v>
-      </c>
-      <c r="B111" t="s">
-        <v>54</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
-      </c>
-      <c r="E111" t="s">
-        <v>55</v>
-      </c>
-      <c r="F111">
-        <v>30</v>
-      </c>
-      <c r="G111" t="s">
-        <v>63</v>
-      </c>
-      <c r="H111" t="s">
-        <v>56</v>
-      </c>
-      <c r="I111" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
-      <c r="A112" t="s">
-        <v>73</v>
-      </c>
-      <c r="B112" t="s">
-        <v>74</v>
-      </c>
-      <c r="D112">
-        <v>1</v>
-      </c>
-      <c r="E112" t="s">
-        <v>75</v>
-      </c>
-      <c r="F112">
-        <v>50</v>
-      </c>
-      <c r="G112" t="s">
-        <v>63</v>
-      </c>
-      <c r="H112" t="s">
-        <v>34</v>
-      </c>
-      <c r="I112" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
-      <c r="A113" t="s">
-        <v>30</v>
-      </c>
-      <c r="B113" t="s">
-        <v>76</v>
-      </c>
-      <c r="C113" t="s">
-        <v>77</v>
-      </c>
-      <c r="D113">
-        <v>1</v>
-      </c>
-      <c r="E113" t="s">
-        <v>78</v>
-      </c>
-      <c r="F113">
-        <v>50</v>
-      </c>
-      <c r="G113" t="s">
-        <v>63</v>
-      </c>
-      <c r="H113" t="s">
-        <v>39</v>
-      </c>
-      <c r="I113" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
-      <c r="A114" t="s">
-        <v>62</v>
-      </c>
-      <c r="B114" t="s">
-        <v>41</v>
-      </c>
-      <c r="D114">
-        <v>3</v>
-      </c>
-      <c r="E114" t="s">
-        <v>17</v>
-      </c>
-      <c r="F114">
-        <v>100</v>
-      </c>
-      <c r="G114" t="s">
-        <v>79</v>
-      </c>
-      <c r="H114" t="s">
-        <v>13</v>
-      </c>
-      <c r="I114" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
-      <c r="A115" t="s">
-        <v>47</v>
-      </c>
-      <c r="B115" t="s">
-        <v>48</v>
-      </c>
-      <c r="D115">
-        <v>6</v>
-      </c>
-      <c r="E115" t="s">
-        <v>70</v>
-      </c>
-      <c r="F115">
-        <v>40</v>
-      </c>
-      <c r="G115" t="s">
-        <v>79</v>
-      </c>
-      <c r="H115" t="s">
-        <v>43</v>
-      </c>
-      <c r="I115" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
-      <c r="A116" t="s">
-        <v>80</v>
-      </c>
-      <c r="B116" t="s">
-        <v>81</v>
-      </c>
-      <c r="D116">
-        <v>2</v>
-      </c>
-      <c r="E116" t="s">
-        <v>82</v>
-      </c>
-      <c r="F116">
-        <v>40</v>
-      </c>
-      <c r="G116" t="s">
-        <v>79</v>
-      </c>
-      <c r="H116" t="s">
-        <v>18</v>
-      </c>
-      <c r="I116" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
-      <c r="A117" t="s">
-        <v>27</v>
-      </c>
-      <c r="B117" t="s">
-        <v>28</v>
-      </c>
-      <c r="D117">
-        <v>1</v>
-      </c>
-      <c r="E117" t="s">
-        <v>83</v>
-      </c>
-      <c r="F117">
-        <v>50</v>
-      </c>
-      <c r="G117" t="s">
-        <v>79</v>
-      </c>
-      <c r="H117" t="s">
-        <v>26</v>
-      </c>
-      <c r="I117" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
-      <c r="A118" t="s">
-        <v>84</v>
-      </c>
-      <c r="B118" t="s">
-        <v>85</v>
-      </c>
-      <c r="C118" t="s">
-        <v>86</v>
-      </c>
-      <c r="D118">
-        <v>1</v>
-      </c>
-      <c r="E118" t="s">
-        <v>55</v>
-      </c>
-      <c r="F118">
-        <v>40</v>
-      </c>
-      <c r="G118" t="s">
-        <v>79</v>
-      </c>
-      <c r="H118" t="s">
-        <v>22</v>
-      </c>
-      <c r="I118" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="A119" t="s">
-        <v>87</v>
-      </c>
-      <c r="B119" t="s">
-        <v>88</v>
-      </c>
-      <c r="C119" t="s">
-        <v>89</v>
-      </c>
-      <c r="D119">
-        <v>1</v>
-      </c>
-      <c r="E119" t="s">
-        <v>90</v>
-      </c>
-      <c r="F119">
-        <v>50</v>
-      </c>
-      <c r="G119" t="s">
-        <v>79</v>
-      </c>
-      <c r="H119" t="s">
-        <v>29</v>
-      </c>
-      <c r="I119" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
-      <c r="A120" t="s">
-        <v>91</v>
-      </c>
-      <c r="B120" t="s">
-        <v>92</v>
-      </c>
-      <c r="D120">
-        <v>1</v>
-      </c>
-      <c r="E120" t="s">
-        <v>21</v>
-      </c>
-      <c r="F120">
-        <v>30</v>
-      </c>
-      <c r="G120" t="s">
-        <v>93</v>
-      </c>
-      <c r="H120" t="s">
-        <v>56</v>
-      </c>
-      <c r="I120" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
-      <c r="A121" t="s">
-        <v>47</v>
-      </c>
-      <c r="B121" t="s">
-        <v>48</v>
-      </c>
-      <c r="D121">
-        <v>1</v>
-      </c>
-      <c r="E121" t="s">
-        <v>94</v>
-      </c>
-      <c r="F121">
-        <v>40</v>
-      </c>
-      <c r="G121" t="s">
-        <v>93</v>
-      </c>
-      <c r="H121" t="s">
-        <v>43</v>
-      </c>
-      <c r="I121" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
-      <c r="A122" t="s">
-        <v>95</v>
-      </c>
-      <c r="B122" t="s">
-        <v>36</v>
-      </c>
-      <c r="D122">
-        <v>3</v>
-      </c>
-      <c r="E122" t="s">
-        <v>94</v>
-      </c>
-      <c r="F122">
-        <v>40</v>
-      </c>
-      <c r="G122" t="s">
-        <v>93</v>
-      </c>
-      <c r="H122" t="s">
-        <v>18</v>
-      </c>
-      <c r="I122" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
-      <c r="A123" t="s">
-        <v>19</v>
-      </c>
-      <c r="B123" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123">
-        <v>5</v>
-      </c>
-      <c r="E123" t="s">
-        <v>21</v>
-      </c>
-      <c r="F123">
-        <v>40</v>
-      </c>
-      <c r="G123" t="s">
-        <v>96</v>
-      </c>
-      <c r="H123" t="s">
-        <v>43</v>
-      </c>
-      <c r="I123" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
-      <c r="A124" t="s">
-        <v>97</v>
-      </c>
-      <c r="B124" t="s">
-        <v>98</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
-      </c>
-      <c r="E124" t="s">
-        <v>21</v>
-      </c>
-      <c r="F124">
-        <v>40</v>
-      </c>
-      <c r="G124" t="s">
-        <v>99</v>
-      </c>
-      <c r="H124" t="s">
-        <v>43</v>
-      </c>
-      <c r="I124" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
-      <c r="A125" t="s">
-        <v>97</v>
-      </c>
-      <c r="B125" t="s">
-        <v>98</v>
-      </c>
-      <c r="D125">
-        <v>3</v>
-      </c>
-      <c r="E125" t="s">
-        <v>21</v>
-      </c>
-      <c r="F125">
-        <v>40</v>
-      </c>
-      <c r="G125" t="s">
-        <v>99</v>
-      </c>
-      <c r="H125" t="s">
-        <v>18</v>
-      </c>
-      <c r="I125" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
-      <c r="A126" t="s">
-        <v>15</v>
-      </c>
-      <c r="B126" t="s">
-        <v>16</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126" t="s">
-        <v>100</v>
-      </c>
-      <c r="F126">
-        <v>80</v>
-      </c>
-      <c r="G126" t="s">
-        <v>99</v>
-      </c>
-      <c r="H126" t="s">
-        <v>13</v>
-      </c>
-      <c r="I126" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
-      <c r="A127" t="s">
-        <v>15</v>
-      </c>
-      <c r="B127" t="s">
-        <v>16</v>
-      </c>
-      <c r="D127">
-        <v>2</v>
-      </c>
-      <c r="E127" t="s">
-        <v>21</v>
-      </c>
-      <c r="F127">
-        <v>80</v>
-      </c>
-      <c r="G127" t="s">
-        <v>99</v>
-      </c>
-      <c r="H127" t="s">
-        <v>64</v>
-      </c>
-      <c r="I127" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="A128" t="s">
-        <v>19</v>
-      </c>
-      <c r="B128" t="s">
-        <v>20</v>
-      </c>
-      <c r="D128">
-        <v>1</v>
-      </c>
-      <c r="E128" t="s">
-        <v>21</v>
-      </c>
-      <c r="F128">
-        <v>40</v>
-      </c>
-      <c r="G128" t="s">
-        <v>99</v>
-      </c>
-      <c r="H128" t="s">
-        <v>22</v>
-      </c>
-      <c r="I128" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
-      <c r="A129" t="s">
-        <v>19</v>
-      </c>
-      <c r="B129" t="s">
-        <v>20</v>
-      </c>
-      <c r="D129">
-        <v>2</v>
-      </c>
-      <c r="E129" t="s">
-        <v>21</v>
-      </c>
-      <c r="F129">
-        <v>40</v>
-      </c>
-      <c r="G129" t="s">
-        <v>99</v>
-      </c>
-      <c r="H129" t="s">
-        <v>23</v>
-      </c>
-      <c r="I129" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
-      <c r="A130" t="s">
-        <v>19</v>
-      </c>
-      <c r="B130" t="s">
-        <v>20</v>
-      </c>
-      <c r="D130">
-        <v>6</v>
-      </c>
-      <c r="E130" t="s">
-        <v>21</v>
-      </c>
-      <c r="F130">
-        <v>40</v>
-      </c>
-      <c r="G130" t="s">
-        <v>99</v>
-      </c>
-      <c r="H130" t="s">
-        <v>26</v>
-      </c>
-      <c r="I130" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
-      <c r="A131" t="s">
-        <v>50</v>
-      </c>
-      <c r="B131" t="s">
-        <v>51</v>
-      </c>
-      <c r="D131">
-        <v>3</v>
-      </c>
-      <c r="E131" t="s">
-        <v>21</v>
-      </c>
-      <c r="F131">
-        <v>40</v>
-      </c>
-      <c r="G131" t="s">
-        <v>99</v>
-      </c>
-      <c r="H131" t="s">
-        <v>29</v>
-      </c>
-      <c r="I131" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
-      <c r="A132" t="s">
-        <v>53</v>
-      </c>
-      <c r="B132" t="s">
-        <v>54</v>
-      </c>
-      <c r="D132">
-        <v>3</v>
-      </c>
-      <c r="E132" t="s">
-        <v>21</v>
-      </c>
-      <c r="F132">
-        <v>30</v>
-      </c>
-      <c r="G132" t="s">
-        <v>99</v>
-      </c>
-      <c r="H132" t="s">
-        <v>56</v>
-      </c>
-      <c r="I132" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
-      <c r="A133" t="s">
-        <v>101</v>
-      </c>
-      <c r="B133" t="s">
-        <v>102</v>
-      </c>
-      <c r="D133">
-        <v>1</v>
-      </c>
-      <c r="E133" t="s">
-        <v>21</v>
-      </c>
-      <c r="F133">
-        <v>50</v>
-      </c>
-      <c r="G133" t="s">
-        <v>99</v>
-      </c>
-      <c r="H133" t="s">
-        <v>34</v>
-      </c>
-      <c r="I133" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
-      <c r="A134" t="s">
-        <v>103</v>
-      </c>
-      <c r="B134" t="s">
-        <v>104</v>
-      </c>
-      <c r="D134">
-        <v>1</v>
-      </c>
-      <c r="E134" t="s">
-        <v>105</v>
-      </c>
-      <c r="F134">
-        <v>50</v>
-      </c>
-      <c r="G134" t="s">
-        <v>99</v>
-      </c>
-      <c r="H134" t="s">
-        <v>39</v>
-      </c>
-      <c r="I134" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
-      <c r="A135" t="s">
-        <v>106</v>
-      </c>
-      <c r="B135" t="s">
-        <v>51</v>
-      </c>
-      <c r="D135">
-        <v>2</v>
-      </c>
-      <c r="E135" t="s">
-        <v>21</v>
-      </c>
-      <c r="F135">
-        <v>50</v>
-      </c>
-      <c r="G135" t="s">
-        <v>99</v>
-      </c>
-      <c r="H135" t="s">
-        <v>107</v>
-      </c>
-      <c r="I135" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
-      <c r="A136" t="s">
-        <v>62</v>
-      </c>
-      <c r="B136" t="s">
-        <v>41</v>
-      </c>
-      <c r="D136">
-        <v>2</v>
-      </c>
-      <c r="E136" t="s">
-        <v>70</v>
-      </c>
-      <c r="F136">
-        <v>100</v>
-      </c>
-      <c r="G136" t="s">
-        <v>108</v>
-      </c>
-      <c r="H136" t="s">
-        <v>13</v>
-      </c>
-      <c r="I136" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
-      <c r="A137" t="s">
-        <v>15</v>
-      </c>
-      <c r="B137" t="s">
-        <v>16</v>
-      </c>
-      <c r="D137">
-        <v>5</v>
-      </c>
-      <c r="E137" t="s">
-        <v>109</v>
-      </c>
-      <c r="F137">
-        <v>40</v>
-      </c>
-      <c r="G137" t="s">
-        <v>108</v>
-      </c>
-      <c r="H137" t="s">
-        <v>43</v>
-      </c>
-      <c r="I137" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
-      <c r="A138" t="s">
-        <v>44</v>
-      </c>
-      <c r="B138" t="s">
-        <v>45</v>
-      </c>
-      <c r="D138">
-        <v>1</v>
-      </c>
-      <c r="E138" t="s">
-        <v>46</v>
-      </c>
-      <c r="F138">
-        <v>40</v>
-      </c>
-      <c r="G138" t="s">
-        <v>108</v>
-      </c>
-      <c r="H138" t="s">
-        <v>18</v>
-      </c>
-      <c r="I138" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
-      <c r="A139" t="s">
-        <v>24</v>
-      </c>
-      <c r="B139" t="s">
-        <v>25</v>
-      </c>
-      <c r="D139">
-        <v>1</v>
-      </c>
-      <c r="E139" t="s">
-        <v>21</v>
-      </c>
-      <c r="F139">
-        <v>40</v>
-      </c>
-      <c r="G139" t="s">
-        <v>108</v>
-      </c>
-      <c r="H139" t="s">
-        <v>22</v>
-      </c>
-      <c r="I139" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
-      <c r="A140" t="s">
-        <v>57</v>
-      </c>
-      <c r="B140" t="s">
-        <v>58</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
-      </c>
-      <c r="E140" t="s">
-        <v>110</v>
-      </c>
-      <c r="F140">
-        <v>40</v>
-      </c>
-      <c r="G140" t="s">
-        <v>108</v>
-      </c>
-      <c r="H140" t="s">
-        <v>23</v>
-      </c>
-      <c r="I140" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
-      <c r="A141" t="s">
-        <v>101</v>
-      </c>
-      <c r="B141" t="s">
-        <v>102</v>
-      </c>
-      <c r="D141">
-        <v>2</v>
-      </c>
-      <c r="E141" t="s">
-        <v>83</v>
-      </c>
-      <c r="F141">
-        <v>50</v>
-      </c>
-      <c r="G141" t="s">
-        <v>108</v>
-      </c>
-      <c r="H141" t="s">
-        <v>26</v>
-      </c>
-      <c r="I141" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9">
-      <c r="A142" t="s">
-        <v>9</v>
-      </c>
-      <c r="B142" t="s">
-        <v>10</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
-      </c>
-      <c r="E142" t="s">
-        <v>65</v>
-      </c>
-      <c r="F142">
-        <v>100</v>
-      </c>
-      <c r="G142" t="s">
-        <v>111</v>
-      </c>
-      <c r="H142" t="s">
-        <v>13</v>
-      </c>
-      <c r="I142" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9">
-      <c r="A143" t="s">
-        <v>15</v>
-      </c>
-      <c r="B143" t="s">
-        <v>16</v>
-      </c>
-      <c r="D143">
-        <v>4</v>
-      </c>
-      <c r="E143" t="s">
-        <v>109</v>
-      </c>
-      <c r="F143">
-        <v>40</v>
-      </c>
-      <c r="G143" t="s">
-        <v>111</v>
-      </c>
-      <c r="H143" t="s">
-        <v>43</v>
-      </c>
-      <c r="I143" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
-      <c r="A144" t="s">
-        <v>67</v>
-      </c>
-      <c r="B144" t="s">
-        <v>68</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
-      </c>
-      <c r="E144" t="s">
-        <v>69</v>
-      </c>
-      <c r="F144">
-        <v>40</v>
-      </c>
-      <c r="G144" t="s">
-        <v>111</v>
-      </c>
-      <c r="H144" t="s">
-        <v>18</v>
-      </c>
-      <c r="I144" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9">
-      <c r="A145" t="s">
-        <v>95</v>
-      </c>
-      <c r="B145" t="s">
-        <v>36</v>
-      </c>
-      <c r="D145">
-        <v>2</v>
-      </c>
-      <c r="E145" t="s">
-        <v>112</v>
-      </c>
-      <c r="F145">
-        <v>40</v>
-      </c>
-      <c r="G145" t="s">
-        <v>111</v>
-      </c>
-      <c r="H145" t="s">
-        <v>22</v>
-      </c>
-      <c r="I145" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9">
-      <c r="A146" t="s">
-        <v>113</v>
-      </c>
-      <c r="B146" t="s">
-        <v>114</v>
-      </c>
-      <c r="D146">
-        <v>1</v>
-      </c>
-      <c r="E146" t="s">
-        <v>115</v>
-      </c>
-      <c r="F146">
-        <v>50</v>
-      </c>
-      <c r="G146" t="s">
-        <v>111</v>
-      </c>
-      <c r="H146" t="s">
-        <v>26</v>
-      </c>
-      <c r="I146" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
-      <c r="A147" t="s">
-        <v>9</v>
-      </c>
-      <c r="B147" t="s">
-        <v>10</v>
-      </c>
-      <c r="D147">
-        <v>3</v>
-      </c>
-      <c r="E147" t="s">
-        <v>69</v>
-      </c>
-      <c r="F147">
-        <v>100</v>
-      </c>
-      <c r="G147" t="s">
-        <v>116</v>
-      </c>
-      <c r="H147" t="s">
-        <v>13</v>
-      </c>
-      <c r="I147" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9">
-      <c r="A148" t="s">
-        <v>47</v>
-      </c>
-      <c r="B148" t="s">
-        <v>48</v>
-      </c>
-      <c r="D148">
-        <v>3</v>
-      </c>
-      <c r="E148" t="s">
-        <v>100</v>
-      </c>
-      <c r="F148">
-        <v>40</v>
-      </c>
-      <c r="G148" t="s">
-        <v>116</v>
-      </c>
-      <c r="H148" t="s">
-        <v>43</v>
-      </c>
-      <c r="I148" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9">
-      <c r="A149" t="s">
-        <v>117</v>
-      </c>
-      <c r="B149" t="s">
-        <v>51</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="E149" t="s">
-        <v>82</v>
-      </c>
-      <c r="F149">
-        <v>40</v>
-      </c>
-      <c r="G149" t="s">
-        <v>116</v>
-      </c>
-      <c r="H149" t="s">
-        <v>18</v>
-      </c>
-      <c r="I149" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9">
-      <c r="A150" t="s">
-        <v>24</v>
-      </c>
-      <c r="B150" t="s">
-        <v>25</v>
-      </c>
-      <c r="D150">
-        <v>2</v>
-      </c>
-      <c r="E150" t="s">
-        <v>118</v>
-      </c>
-      <c r="F150">
-        <v>40</v>
-      </c>
-      <c r="G150" t="s">
-        <v>116</v>
-      </c>
-      <c r="H150" t="s">
-        <v>22</v>
-      </c>
-      <c r="I150" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
-      <c r="A151" t="s">
-        <v>119</v>
-      </c>
-      <c r="B151" t="s">
-        <v>120</v>
-      </c>
-      <c r="D151">
-        <v>1</v>
-      </c>
-      <c r="E151" t="s">
-        <v>121</v>
-      </c>
-      <c r="F151">
-        <v>50</v>
-      </c>
-      <c r="G151" t="s">
-        <v>116</v>
-      </c>
-      <c r="H151" t="s">
-        <v>26</v>
-      </c>
-      <c r="I151" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
-      <c r="A152" t="s">
-        <v>122</v>
-      </c>
-      <c r="B152" t="s">
-        <v>102</v>
-      </c>
-      <c r="D152">
-        <v>1</v>
-      </c>
-      <c r="E152" t="s">
-        <v>123</v>
-      </c>
-      <c r="F152">
-        <v>50</v>
-      </c>
-      <c r="G152" t="s">
-        <v>116</v>
-      </c>
-      <c r="H152" t="s">
-        <v>29</v>
-      </c>
-      <c r="I152" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9">
-      <c r="A153" t="s">
-        <v>9</v>
-      </c>
-      <c r="B153" t="s">
-        <v>10</v>
-      </c>
-      <c r="D153">
-        <v>4</v>
-      </c>
-      <c r="E153" t="s">
-        <v>69</v>
-      </c>
-      <c r="F153">
-        <v>100</v>
-      </c>
-      <c r="G153" t="s">
-        <v>124</v>
-      </c>
-      <c r="H153" t="s">
-        <v>13</v>
-      </c>
-      <c r="I153" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
-      <c r="A154" t="s">
-        <v>44</v>
-      </c>
-      <c r="B154" t="s">
-        <v>45</v>
-      </c>
-      <c r="D154">
-        <v>2</v>
-      </c>
-      <c r="E154" t="s">
-        <v>46</v>
-      </c>
-      <c r="F154">
-        <v>40</v>
-      </c>
-      <c r="G154" t="s">
-        <v>124</v>
-      </c>
-      <c r="H154" t="s">
-        <v>43</v>
-      </c>
-      <c r="I154" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
-      <c r="A155" t="s">
-        <v>67</v>
-      </c>
-      <c r="B155" t="s">
-        <v>68</v>
-      </c>
-      <c r="D155">
-        <v>4</v>
-      </c>
-      <c r="E155" t="s">
-        <v>83</v>
-      </c>
-      <c r="F155">
-        <v>40</v>
-      </c>
-      <c r="G155" t="s">
-        <v>124</v>
-      </c>
-      <c r="H155" t="s">
-        <v>18</v>
-      </c>
-      <c r="I155" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9">
-      <c r="A156" t="s">
-        <v>125</v>
-      </c>
-      <c r="B156" t="s">
-        <v>126</v>
-      </c>
-      <c r="D156">
-        <v>3</v>
-      </c>
-      <c r="E156" t="s">
-        <v>21</v>
-      </c>
-      <c r="F156">
-        <v>40</v>
-      </c>
-      <c r="G156" t="s">
-        <v>124</v>
-      </c>
-      <c r="H156" t="s">
-        <v>22</v>
-      </c>
-      <c r="I156" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
-      <c r="A157" t="s">
-        <v>27</v>
-      </c>
-      <c r="B157" t="s">
-        <v>28</v>
-      </c>
-      <c r="D157">
-        <v>2</v>
-      </c>
-      <c r="E157" t="s">
-        <v>127</v>
-      </c>
-      <c r="F157">
-        <v>50</v>
-      </c>
-      <c r="G157" t="s">
-        <v>124</v>
-      </c>
-      <c r="H157" t="s">
-        <v>26</v>
-      </c>
-      <c r="I157" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9">
-      <c r="A158" t="s">
-        <v>128</v>
-      </c>
-      <c r="B158" t="s">
-        <v>129</v>
-      </c>
-      <c r="D158">
-        <v>1</v>
-      </c>
-      <c r="E158" t="s">
-        <v>130</v>
-      </c>
-      <c r="F158">
-        <v>50</v>
-      </c>
-      <c r="G158" t="s">
-        <v>124</v>
-      </c>
-      <c r="H158" t="s">
-        <v>29</v>
-      </c>
-      <c r="I158" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9">
-      <c r="A159" t="s">
-        <v>30</v>
-      </c>
-      <c r="B159" t="s">
-        <v>131</v>
-      </c>
-      <c r="C159" t="s">
-        <v>77</v>
-      </c>
-      <c r="D159">
-        <v>1</v>
-      </c>
-      <c r="E159" t="s">
-        <v>132</v>
-      </c>
-      <c r="F159">
-        <v>50</v>
-      </c>
-      <c r="G159" t="s">
-        <v>124</v>
-      </c>
-      <c r="H159" t="s">
-        <v>34</v>
-      </c>
-      <c r="I159" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9">
-      <c r="A160" t="s">
-        <v>106</v>
-      </c>
-      <c r="B160" t="s">
-        <v>51</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
-      </c>
-      <c r="E160" t="s">
-        <v>133</v>
-      </c>
-      <c r="F160">
-        <v>50</v>
-      </c>
-      <c r="G160" t="s">
-        <v>124</v>
-      </c>
-      <c r="H160" t="s">
-        <v>39</v>
-      </c>
-      <c r="I160" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9">
-      <c r="A161" t="s">
-        <v>19</v>
-      </c>
-      <c r="B161" t="s">
-        <v>20</v>
-      </c>
-      <c r="D161">
-        <v>3</v>
-      </c>
-      <c r="E161" t="s">
-        <v>21</v>
-      </c>
-      <c r="F161">
-        <v>40</v>
-      </c>
-      <c r="G161" t="s">
-        <v>134</v>
-      </c>
-      <c r="H161" t="s">
-        <v>43</v>
-      </c>
-      <c r="I161" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9">
-      <c r="A162" t="s">
-        <v>53</v>
-      </c>
-      <c r="B162" t="s">
-        <v>54</v>
-      </c>
-      <c r="D162">
-        <v>4</v>
-      </c>
-      <c r="E162" t="s">
-        <v>21</v>
-      </c>
-      <c r="F162">
-        <v>30</v>
-      </c>
-      <c r="G162" t="s">
-        <v>134</v>
-      </c>
-      <c r="H162" t="s">
-        <v>56</v>
-      </c>
-      <c r="I162" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9">
-      <c r="A163" t="s">
-        <v>87</v>
-      </c>
-      <c r="B163" t="s">
-        <v>135</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="E163" t="s">
-        <v>130</v>
-      </c>
-      <c r="F163">
-        <v>50</v>
-      </c>
-      <c r="G163" t="s">
-        <v>134</v>
-      </c>
-      <c r="H163" t="s">
-        <v>26</v>
-      </c>
-      <c r="I163" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
-      <c r="A164" t="s">
-        <v>136</v>
-      </c>
-      <c r="B164" t="s">
-        <v>137</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-      <c r="E164" t="s">
-        <v>138</v>
-      </c>
-      <c r="F164">
-        <v>50</v>
-      </c>
-      <c r="G164" t="s">
-        <v>134</v>
-      </c>
-      <c r="H164" t="s">
-        <v>29</v>
-      </c>
-      <c r="I164" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9">
-      <c r="A165" t="s">
-        <v>67</v>
-      </c>
-      <c r="B165" t="s">
-        <v>68</v>
-      </c>
-      <c r="D165">
-        <v>2</v>
-      </c>
-      <c r="E165" t="s">
-        <v>83</v>
-      </c>
-      <c r="F165">
-        <v>40</v>
-      </c>
-      <c r="G165" t="s">
-        <v>139</v>
-      </c>
-      <c r="H165" t="s">
-        <v>43</v>
-      </c>
-      <c r="I165" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9">
-      <c r="A166" t="s">
-        <v>47</v>
-      </c>
-      <c r="B166" t="s">
-        <v>48</v>
-      </c>
-      <c r="D166">
-        <v>2</v>
-      </c>
-      <c r="E166" t="s">
-        <v>100</v>
-      </c>
-      <c r="F166">
-        <v>40</v>
-      </c>
-      <c r="G166" t="s">
-        <v>139</v>
-      </c>
-      <c r="H166" t="s">
-        <v>18</v>
-      </c>
-      <c r="I166" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9">
-      <c r="A167" t="s">
-        <v>125</v>
-      </c>
-      <c r="B167" t="s">
-        <v>126</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-      <c r="E167" t="s">
-        <v>21</v>
-      </c>
-      <c r="F167">
-        <v>40</v>
-      </c>
-      <c r="G167" t="s">
-        <v>139</v>
-      </c>
-      <c r="H167" t="s">
-        <v>22</v>
-      </c>
-      <c r="I167" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
-      <c r="A168" t="s">
-        <v>95</v>
-      </c>
-      <c r="B168" t="s">
-        <v>36</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168" t="s">
-        <v>112</v>
-      </c>
-      <c r="F168">
-        <v>40</v>
-      </c>
-      <c r="G168" t="s">
-        <v>139</v>
-      </c>
-      <c r="H168" t="s">
-        <v>23</v>
-      </c>
-      <c r="I168" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9">
-      <c r="A169" t="s">
-        <v>140</v>
-      </c>
-      <c r="B169" t="s">
-        <v>141</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-      <c r="E169" t="s">
-        <v>142</v>
-      </c>
-      <c r="F169">
-        <v>50</v>
-      </c>
-      <c r="G169" t="s">
-        <v>139</v>
-      </c>
-      <c r="H169" t="s">
-        <v>26</v>
-      </c>
-      <c r="I169" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
-      <c r="A170" t="s">
-        <v>143</v>
-      </c>
-      <c r="B170" t="s">
-        <v>25</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-      <c r="E170" t="s">
-        <v>110</v>
-      </c>
-      <c r="F170">
-        <v>50</v>
-      </c>
-      <c r="G170" t="s">
-        <v>139</v>
-      </c>
-      <c r="H170" t="s">
-        <v>29</v>
-      </c>
-      <c r="I170" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
-      <c r="A171" t="s">
-        <v>35</v>
-      </c>
-      <c r="B171" t="s">
-        <v>36</v>
-      </c>
-      <c r="D171">
-        <v>1</v>
-      </c>
-      <c r="E171" t="s">
-        <v>37</v>
-      </c>
-      <c r="F171">
-        <v>50</v>
-      </c>
-      <c r="G171" t="s">
-        <v>38</v>
-      </c>
-      <c r="H171" t="s">
-        <v>39</v>
-      </c>
-      <c r="I171" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
-      <c r="A172" t="s">
-        <v>144</v>
-      </c>
-      <c r="B172" t="s">
-        <v>145</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172" t="s">
-        <v>21</v>
-      </c>
-      <c r="F172">
-        <v>50</v>
-      </c>
-      <c r="I172" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9">
-      <c r="A173" t="s">
-        <v>144</v>
-      </c>
-      <c r="B173" t="s">
-        <v>145</v>
-      </c>
-      <c r="D173">
-        <v>2</v>
-      </c>
-      <c r="E173" t="s">
-        <v>130</v>
-      </c>
-      <c r="F173">
-        <v>50</v>
-      </c>
-      <c r="I173" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9">
-      <c r="A174" t="s">
-        <v>59</v>
-      </c>
-      <c r="B174" t="s">
-        <v>60</v>
-      </c>
-      <c r="D174">
-        <v>2</v>
-      </c>
-      <c r="E174" t="s">
-        <v>21</v>
-      </c>
-      <c r="F174">
-        <v>40</v>
-      </c>
-      <c r="I174" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9">
-      <c r="A175" t="s">
-        <v>30</v>
-      </c>
-      <c r="B175" t="s">
-        <v>147</v>
-      </c>
-      <c r="D175">
-        <v>1</v>
-      </c>
-      <c r="E175" t="s">
-        <v>21</v>
-      </c>
-      <c r="F175">
-        <v>50</v>
-      </c>
-      <c r="I175" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added buttons to scheduler
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="145">
   <si>
     <t>Course</t>
   </si>
@@ -320,102 +320,105 @@
     <t>Wilson, Marcella</t>
   </si>
   <si>
+    <t>CMSC 483/691</t>
+  </si>
+  <si>
+    <t>Parallel &amp; Distr. Processing</t>
+  </si>
+  <si>
+    <t>Simon, Tyler</t>
+  </si>
+  <si>
+    <t>CMSC 682</t>
+  </si>
+  <si>
+    <t>Network Technologies</t>
+  </si>
+  <si>
+    <t>Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>tt1130</t>
+  </si>
+  <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
+    <t>Kalpakis, Kostas</t>
+  </si>
+  <si>
     <t>CMSC 478</t>
   </si>
   <si>
     <t>Machine Learning</t>
   </si>
   <si>
-    <t>CMSC 483/691</t>
-  </si>
-  <si>
-    <t>Parallel &amp; Distr. Processing</t>
-  </si>
-  <si>
-    <t>Simon, Tyler</t>
+    <t>tt10</t>
+  </si>
+  <si>
+    <t>Chang, Richard</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>tt230</t>
+  </si>
+  <si>
+    <t>CMSC 411ce</t>
+  </si>
+  <si>
+    <t>Perkins, Dmitri</t>
+  </si>
+  <si>
+    <t>CMSC 479/679</t>
+  </si>
+  <si>
+    <t>Introduction to Robotics</t>
+  </si>
+  <si>
+    <t>Matuszek, Cynthia</t>
+  </si>
+  <si>
+    <t>CMSC 678</t>
+  </si>
+  <si>
+    <t>Oates, Tim</t>
+  </si>
+  <si>
+    <t>tt4</t>
+  </si>
+  <si>
+    <t>CMSC 426</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>Finin, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 481</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Spec Topic: Computer Vision</t>
+  </si>
+  <si>
+    <t>Chapman, David</t>
   </si>
   <si>
     <t>CMSC 611</t>
   </si>
   <si>
-    <t>Interdisciplinary Life S 237</t>
-  </si>
-  <si>
-    <t>tt1130</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>tt10</t>
-  </si>
-  <si>
-    <t>Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>tt230</t>
-  </si>
-  <si>
-    <t>CMSC 411ce</t>
-  </si>
-  <si>
-    <t>Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 479/679</t>
-  </si>
-  <si>
-    <t>Introduction to Robotics</t>
-  </si>
-  <si>
-    <t>Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 678</t>
-  </si>
-  <si>
-    <t>Oates, Tim</t>
-  </si>
-  <si>
-    <t>tt4</t>
-  </si>
-  <si>
-    <t>CMSC 426</t>
-  </si>
-  <si>
-    <t>Computer Security</t>
-  </si>
-  <si>
-    <t>Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 481</t>
-  </si>
-  <si>
-    <t>Computer Networks</t>
-  </si>
-  <si>
-    <t>Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>Spec Topic: Computer Vision</t>
-  </si>
-  <si>
-    <t>Chapman, David</t>
-  </si>
-  <si>
     <t>Liu, Chenchen</t>
   </si>
   <si>
@@ -447,48 +450,6 @@
   </si>
   <si>
     <t>CMSC 621</t>
-  </si>
-  <si>
-    <t>CMSC 682</t>
-  </si>
-  <si>
-    <t>Network Technologies</t>
-  </si>
-  <si>
-    <t>unscheduled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spec Topic: Internet of Things </t>
-  </si>
-  <si>
-    <t>course</t>
-  </si>
-  <si>
-    <t>alt1</t>
-  </si>
-  <si>
-    <t>alt2</t>
-  </si>
-  <si>
-    <t>alt3</t>
-  </si>
-  <si>
-    <t>CMSC 682Network Technologies2Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>{'mw530': Interdisciplinary Life S 237}</t>
-  </si>
-  <si>
-    <t>{'mw530': Public Policy 105}</t>
-  </si>
-  <si>
-    <t>{'mw230': Sherman Hall 014}</t>
-  </si>
-  <si>
-    <t>CMSC 684Wireless Sensor Networks2Staff</t>
-  </si>
-  <si>
-    <t>CMSC 491/691Spec Topic: Internet of Things 1Staff</t>
   </si>
 </sst>
 </file>
@@ -820,7 +781,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I175"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -889,7 +850,7 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -915,7 +876,7 @@
         <v>20</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -941,7 +902,7 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -1100,7 +1061,7 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -1334,7 +1295,7 @@
         <v>16</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1811,7 +1772,7 @@
         <v>20</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
@@ -1857,25 +1818,25 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="F40">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G40" t="s">
         <v>99</v>
       </c>
       <c r="H40" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I40" t="s">
         <v>14</v>
@@ -1883,25 +1844,25 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F41">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
         <v>99</v>
       </c>
       <c r="H41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I41" t="s">
         <v>14</v>
@@ -1909,25 +1870,25 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
       </c>
       <c r="F42">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G42" t="s">
         <v>99</v>
       </c>
       <c r="H42" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I42" t="s">
         <v>14</v>
@@ -1935,13 +1896,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
         <v>21</v>
@@ -1953,7 +1914,7 @@
         <v>99</v>
       </c>
       <c r="H43" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I43" t="s">
         <v>14</v>
@@ -1961,25 +1922,25 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" t="s">
         <v>21</v>
       </c>
       <c r="F44">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G44" t="s">
         <v>99</v>
       </c>
       <c r="H44" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="I44" t="s">
         <v>14</v>
@@ -1987,19 +1948,19 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="D45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="F45">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s">
         <v>99</v>
@@ -2013,19 +1974,19 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46">
         <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46">
-        <v>40</v>
       </c>
       <c r="G46" t="s">
         <v>99</v>
@@ -2039,25 +2000,25 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F47">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G47" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H47" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I47" t="s">
         <v>14</v>
@@ -2065,25 +2026,25 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="F48">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G48" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H48" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I48" t="s">
         <v>14</v>
@@ -2091,25 +2052,25 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
       <c r="F49">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G49" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H49" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="I49" t="s">
         <v>14</v>
@@ -2117,25 +2078,25 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>21</v>
       </c>
       <c r="F50">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G50" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H50" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="I50" t="s">
         <v>14</v>
@@ -2143,25 +2104,25 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="F51">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I51" t="s">
         <v>14</v>
@@ -2169,25 +2130,25 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="F52">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H52" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I52" t="s">
         <v>14</v>
@@ -2195,25 +2156,25 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="F53">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H53" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I53" t="s">
         <v>14</v>
@@ -2221,25 +2182,25 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="F54">
         <v>40</v>
       </c>
       <c r="G54" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H54" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I54" t="s">
         <v>14</v>
@@ -2247,25 +2208,25 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="F55">
         <v>40</v>
       </c>
       <c r="G55" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H55" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I55" t="s">
         <v>14</v>
@@ -2273,25 +2234,25 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="F56">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G56" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H56" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I56" t="s">
         <v>14</v>
@@ -2299,25 +2260,25 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="F57">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G57" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H57" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I57" t="s">
         <v>14</v>
@@ -2325,25 +2286,25 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="F58">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G58" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H58" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="I58" t="s">
         <v>14</v>
@@ -2351,25 +2312,25 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="F59">
         <v>40</v>
       </c>
       <c r="G59" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H59" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="I59" t="s">
         <v>14</v>
@@ -2377,25 +2338,25 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="F60">
         <v>40</v>
       </c>
       <c r="G60" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H60" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I60" t="s">
         <v>14</v>
@@ -2403,25 +2364,25 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F61">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G61" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H61" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I61" t="s">
         <v>14</v>
@@ -2429,25 +2390,25 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="F62">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H62" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I62" t="s">
         <v>14</v>
@@ -2455,25 +2416,25 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F63">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H63" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="I63" t="s">
         <v>14</v>
@@ -2481,25 +2442,25 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F64">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G64" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H64" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I64" t="s">
         <v>14</v>
@@ -2507,25 +2468,25 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D65">
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="F65">
         <v>40</v>
       </c>
       <c r="G65" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H65" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I65" t="s">
         <v>14</v>
@@ -2533,25 +2494,25 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="F66">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G66" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H66" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I66" t="s">
         <v>14</v>
@@ -2559,25 +2520,25 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="F67">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G67" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H67" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I67" t="s">
         <v>14</v>
@@ -2585,25 +2546,25 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="F68">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I68" t="s">
         <v>14</v>
@@ -2611,25 +2572,25 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="F69">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G69" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H69" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="I69" t="s">
         <v>14</v>
@@ -2637,25 +2598,28 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C70" t="s">
+        <v>77</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="F70">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G70" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H70" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="I70" t="s">
         <v>14</v>
@@ -2663,25 +2627,25 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>134</v>
+      </c>
+      <c r="F71">
+        <v>50</v>
+      </c>
+      <c r="G71" t="s">
         <v>125</v>
       </c>
-      <c r="B71" t="s">
-        <v>126</v>
-      </c>
-      <c r="D71">
-        <v>3</v>
-      </c>
-      <c r="E71" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71">
-        <v>40</v>
-      </c>
-      <c r="G71" t="s">
-        <v>124</v>
-      </c>
       <c r="H71" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="I71" t="s">
         <v>14</v>
@@ -2689,25 +2653,25 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="F72">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G72" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H72" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I72" t="s">
         <v>14</v>
@@ -2715,25 +2679,25 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="F73">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G73" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H73" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="I73" t="s">
         <v>14</v>
@@ -2741,28 +2705,25 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
-      </c>
-      <c r="C74" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="F74">
         <v>50</v>
       </c>
       <c r="G74" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H74" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I74" t="s">
         <v>14</v>
@@ -2770,25 +2731,25 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F75">
         <v>50</v>
       </c>
       <c r="G75" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H75" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I75" t="s">
         <v>14</v>
@@ -2796,22 +2757,22 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="F76">
         <v>40</v>
       </c>
       <c r="G76" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H76" t="s">
         <v>43</v>
@@ -2822,25 +2783,25 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="F77">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G77" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H77" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="I77" t="s">
         <v>14</v>
@@ -2848,25 +2809,25 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="F78">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G78" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H78" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I78" t="s">
         <v>14</v>
@@ -2874,25 +2835,25 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="B79" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="F79">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H79" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I79" t="s">
         <v>14</v>
@@ -2900,25 +2861,25 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="F80">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G80" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H80" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I80" t="s">
         <v>14</v>
@@ -2926,25 +2887,25 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F81">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G81" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H81" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I81" t="s">
         <v>14</v>
@@ -2952,13 +2913,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
         <v>21</v>
@@ -2967,10 +2928,10 @@
         <v>40</v>
       </c>
       <c r="G82" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="H82" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I82" t="s">
         <v>14</v>
@@ -2978,25 +2939,25 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="F83">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I83" t="s">
         <v>14</v>
@@ -3004,25 +2965,25 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="F84">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="H84" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I84" t="s">
         <v>14</v>
@@ -3030,25 +2991,25 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E85" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="F85">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G85" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="H85" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I85" t="s">
         <v>14</v>
@@ -3056,13 +3017,13 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E86" t="s">
         <v>21</v>
@@ -3074,7 +3035,7 @@
         <v>12</v>
       </c>
       <c r="H86" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="I86" t="s">
         <v>14</v>
@@ -3082,25 +3043,25 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D87">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F87">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G87" t="s">
         <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I87" t="s">
         <v>14</v>
@@ -3108,25 +3069,25 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
       <c r="E88" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F88">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G88" t="s">
         <v>12</v>
       </c>
       <c r="H88" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I88" t="s">
         <v>14</v>
@@ -3134,25 +3095,28 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="C89" t="s">
+        <v>32</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F89">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G89" t="s">
         <v>12</v>
       </c>
       <c r="H89" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I89" t="s">
         <v>14</v>
@@ -3160,25 +3124,25 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B90" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D90">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="F90">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G90" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H90" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I90" t="s">
         <v>14</v>
@@ -3186,25 +3150,25 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E91" t="s">
         <v>21</v>
       </c>
       <c r="F91">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G91" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H91" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I91" t="s">
         <v>14</v>
@@ -3212,25 +3176,25 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E92" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F92">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G92" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H92" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I92" t="s">
         <v>14</v>
@@ -3238,28 +3202,25 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
-      </c>
-      <c r="C93" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F93">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G93" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H93" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I93" t="s">
         <v>14</v>
@@ -3267,25 +3228,25 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B94" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F94">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G94" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H94" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="I94" t="s">
         <v>14</v>
@@ -3293,25 +3254,25 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F95">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G95" t="s">
         <v>42</v>
       </c>
       <c r="H95" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I95" t="s">
         <v>14</v>
@@ -3319,25 +3280,25 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="D96">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="F96">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G96" t="s">
         <v>42</v>
       </c>
       <c r="H96" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="I96" t="s">
         <v>14</v>
@@ -3345,16 +3306,16 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F97">
         <v>40</v>
@@ -3363,7 +3324,7 @@
         <v>42</v>
       </c>
       <c r="H97" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I97" t="s">
         <v>14</v>
@@ -3371,16 +3332,16 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D98">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F98">
         <v>40</v>
@@ -3389,7 +3350,7 @@
         <v>42</v>
       </c>
       <c r="H98" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I98" t="s">
         <v>14</v>
@@ -3397,25 +3358,25 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B99" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F99">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G99" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H99" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="I99" t="s">
         <v>14</v>
@@ -3423,25 +3384,25 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F100">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G100" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H100" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I100" t="s">
         <v>14</v>
@@ -3449,25 +3410,25 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B101" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E101" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F101">
         <v>40</v>
       </c>
       <c r="G101" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H101" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I101" t="s">
         <v>14</v>
@@ -3475,25 +3436,25 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E102" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F102">
         <v>40</v>
       </c>
       <c r="G102" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="H102" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I102" t="s">
         <v>14</v>
@@ -3501,25 +3462,25 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="F103">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G103" t="s">
         <v>63</v>
       </c>
       <c r="H103" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I103" t="s">
         <v>14</v>
@@ -3527,25 +3488,25 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="D104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E104" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F104">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G104" t="s">
         <v>63</v>
       </c>
       <c r="H104" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I104" t="s">
         <v>14</v>
@@ -3553,16 +3514,16 @@
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D105">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F105">
         <v>40</v>
@@ -3571,7 +3532,7 @@
         <v>63</v>
       </c>
       <c r="H105" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I105" t="s">
         <v>14</v>
@@ -3579,25 +3540,25 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B106" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D106">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F106">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G106" t="s">
         <v>63</v>
       </c>
       <c r="H106" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I106" t="s">
         <v>14</v>
@@ -3605,25 +3566,25 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B107" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D107">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F107">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G107" t="s">
         <v>63</v>
       </c>
       <c r="H107" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I107" t="s">
         <v>14</v>
@@ -3631,25 +3592,25 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B108" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D108">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F108">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G108" t="s">
         <v>63</v>
       </c>
       <c r="H108" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I108" t="s">
         <v>14</v>
@@ -3657,25 +3618,28 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C109" t="s">
+        <v>77</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F109">
         <v>50</v>
-      </c>
-      <c r="B109" t="s">
-        <v>51</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
-      </c>
-      <c r="E109" t="s">
-        <v>46</v>
-      </c>
-      <c r="F109">
-        <v>40</v>
       </c>
       <c r="G109" t="s">
         <v>63</v>
       </c>
       <c r="H109" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I109" t="s">
         <v>14</v>
@@ -3683,25 +3647,25 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B110" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E110" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="F110">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G110" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H110" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="I110" t="s">
         <v>14</v>
@@ -3709,25 +3673,25 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B111" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E111" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F111">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G111" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H111" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="I111" t="s">
         <v>14</v>
@@ -3735,25 +3699,25 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B112" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F112">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G112" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H112" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I112" t="s">
         <v>14</v>
@@ -3761,28 +3725,25 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>76</v>
-      </c>
-      <c r="C113" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D113">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F113">
         <v>50</v>
       </c>
       <c r="G113" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H113" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="I113" t="s">
         <v>14</v>
@@ -3790,25 +3751,28 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>85</v>
+      </c>
+      <c r="C114" t="s">
+        <v>86</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="F114">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G114" t="s">
         <v>79</v>
       </c>
       <c r="H114" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I114" t="s">
         <v>14</v>
@@ -3816,25 +3780,28 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B115" t="s">
-        <v>48</v>
+        <v>88</v>
+      </c>
+      <c r="C115" t="s">
+        <v>89</v>
       </c>
       <c r="D115">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F115">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G115" t="s">
         <v>79</v>
       </c>
       <c r="H115" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="I115" t="s">
         <v>14</v>
@@ -3842,25 +3809,25 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B116" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E116" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="F116">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G116" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H116" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="I116" t="s">
         <v>14</v>
@@ -3868,25 +3835,25 @@
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B117" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D117">
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="F117">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G117" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H117" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I117" t="s">
         <v>14</v>
@@ -3894,28 +3861,25 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B118" t="s">
-        <v>85</v>
-      </c>
-      <c r="C118" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E118" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="F118">
         <v>40</v>
       </c>
       <c r="G118" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H118" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I118" t="s">
         <v>14</v>
@@ -3923,28 +3887,25 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>88</v>
-      </c>
-      <c r="C119" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E119" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="F119">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G119" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="H119" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I119" t="s">
         <v>14</v>
@@ -3952,10 +3913,10 @@
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B120" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -3964,13 +3925,13 @@
         <v>21</v>
       </c>
       <c r="F120">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G120" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H120" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="I120" t="s">
         <v>14</v>
@@ -3978,25 +3939,25 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B121" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D121">
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F121">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G121" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H121" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="I121" t="s">
         <v>14</v>
@@ -4004,22 +3965,22 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D122">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E122" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="F122">
         <v>40</v>
       </c>
       <c r="G122" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H122" t="s">
         <v>18</v>
@@ -4045,10 +4006,10 @@
         <v>40</v>
       </c>
       <c r="G123" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H123" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I123" t="s">
         <v>14</v>
@@ -4056,13 +4017,13 @@
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B124" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E124" t="s">
         <v>21</v>
@@ -4074,7 +4035,7 @@
         <v>99</v>
       </c>
       <c r="H124" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="I124" t="s">
         <v>14</v>
@@ -4082,10 +4043,10 @@
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="B125" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="D125">
         <v>3</v>
@@ -4094,13 +4055,13 @@
         <v>21</v>
       </c>
       <c r="F125">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G125" t="s">
         <v>99</v>
       </c>
       <c r="H125" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="I125" t="s">
         <v>14</v>
@@ -4108,25 +4069,25 @@
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="B126" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="D126">
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F126">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G126" t="s">
         <v>99</v>
       </c>
       <c r="H126" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I126" t="s">
         <v>14</v>
@@ -4134,25 +4095,25 @@
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="B127" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="F127">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G127" t="s">
         <v>99</v>
       </c>
       <c r="H127" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="I127" t="s">
         <v>14</v>
@@ -4160,25 +4121,25 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B128" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E128" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F128">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G128" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H128" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I128" t="s">
         <v>14</v>
@@ -4186,25 +4147,25 @@
     </row>
     <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B129" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D129">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E129" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="F129">
         <v>40</v>
       </c>
       <c r="G129" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H129" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I129" t="s">
         <v>14</v>
@@ -4212,25 +4173,25 @@
     </row>
     <row r="130" spans="1:9">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D130">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="F130">
         <v>40</v>
       </c>
       <c r="G130" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H130" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I130" t="s">
         <v>14</v>
@@ -4238,13 +4199,13 @@
     </row>
     <row r="131" spans="1:9">
       <c r="A131" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B131" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D131">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E131" t="s">
         <v>21</v>
@@ -4253,10 +4214,10 @@
         <v>40</v>
       </c>
       <c r="G131" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H131" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I131" t="s">
         <v>14</v>
@@ -4264,25 +4225,25 @@
     </row>
     <row r="132" spans="1:9">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B132" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D132">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E132" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F132">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G132" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H132" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="I132" t="s">
         <v>14</v>
@@ -4290,25 +4251,25 @@
     </row>
     <row r="133" spans="1:9">
       <c r="A133" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B133" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D133">
         <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="F133">
         <v>50</v>
       </c>
       <c r="G133" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H133" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I133" t="s">
         <v>14</v>
@@ -4316,25 +4277,25 @@
     </row>
     <row r="134" spans="1:9">
       <c r="A134" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="D134">
         <v>1</v>
       </c>
       <c r="E134" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="F134">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G134" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="H134" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="I134" t="s">
         <v>14</v>
@@ -4342,25 +4303,25 @@
     </row>
     <row r="135" spans="1:9">
       <c r="A135" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="B135" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="D135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="F135">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G135" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="H135" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="I135" t="s">
         <v>14</v>
@@ -4368,25 +4329,25 @@
     </row>
     <row r="136" spans="1:9">
       <c r="A136" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B136" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E136" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F136">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G136" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H136" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I136" t="s">
         <v>14</v>
@@ -4394,25 +4355,25 @@
     </row>
     <row r="137" spans="1:9">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D137">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F137">
         <v>40</v>
       </c>
       <c r="G137" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H137" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I137" t="s">
         <v>14</v>
@@ -4420,25 +4381,25 @@
     </row>
     <row r="138" spans="1:9">
       <c r="A138" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B138" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="D138">
         <v>1</v>
       </c>
       <c r="E138" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="F138">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G138" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H138" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I138" t="s">
         <v>14</v>
@@ -4446,25 +4407,25 @@
     </row>
     <row r="139" spans="1:9">
       <c r="A139" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D139">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E139" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="F139">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G139" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H139" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I139" t="s">
         <v>14</v>
@@ -4472,25 +4433,25 @@
     </row>
     <row r="140" spans="1:9">
       <c r="A140" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B140" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E140" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F140">
         <v>40</v>
       </c>
       <c r="G140" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H140" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="I140" t="s">
         <v>14</v>
@@ -4498,25 +4459,25 @@
     </row>
     <row r="141" spans="1:9">
       <c r="A141" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B141" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="D141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F141">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G141" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H141" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I141" t="s">
         <v>14</v>
@@ -4524,25 +4485,25 @@
     </row>
     <row r="142" spans="1:9">
       <c r="A142" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D142">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E142" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="F142">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G142" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H142" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I142" t="s">
         <v>14</v>
@@ -4550,25 +4511,25 @@
     </row>
     <row r="143" spans="1:9">
       <c r="A143" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="B143" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="D143">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F143">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G143" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H143" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I143" t="s">
         <v>14</v>
@@ -4576,25 +4537,25 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B144" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="D144">
         <v>1</v>
       </c>
       <c r="E144" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="F144">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G144" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H144" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I144" t="s">
         <v>14</v>
@@ -4602,25 +4563,25 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E145" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="F145">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G145" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="H145" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I145" t="s">
         <v>14</v>
@@ -4628,25 +4589,25 @@
     </row>
     <row r="146" spans="1:9">
       <c r="A146" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="B146" t="s">
-        <v>114</v>
+        <v>45</v>
       </c>
       <c r="D146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E146" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
       <c r="F146">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G146" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="H146" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I146" t="s">
         <v>14</v>
@@ -4654,25 +4615,25 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="B147" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D147">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E147" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F147">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G147" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H147" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I147" t="s">
         <v>14</v>
@@ -4680,25 +4641,25 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="B148" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="D148">
         <v>3</v>
       </c>
       <c r="E148" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="F148">
         <v>40</v>
       </c>
       <c r="G148" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H148" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I148" t="s">
         <v>14</v>
@@ -4706,25 +4667,25 @@
     </row>
     <row r="149" spans="1:9">
       <c r="A149" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B149" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D149">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E149" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="F149">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G149" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H149" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I149" t="s">
         <v>14</v>
@@ -4732,25 +4693,25 @@
     </row>
     <row r="150" spans="1:9">
       <c r="A150" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E150" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F150">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G150" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H150" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I150" t="s">
         <v>14</v>
@@ -4758,25 +4719,28 @@
     </row>
     <row r="151" spans="1:9">
       <c r="A151" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="B151" t="s">
-        <v>120</v>
+        <v>131</v>
+      </c>
+      <c r="C151" t="s">
+        <v>77</v>
       </c>
       <c r="D151">
         <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="F151">
         <v>50</v>
       </c>
       <c r="G151" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H151" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I151" t="s">
         <v>14</v>
@@ -4784,25 +4748,25 @@
     </row>
     <row r="152" spans="1:9">
       <c r="A152" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B152" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="D152">
         <v>1</v>
       </c>
       <c r="E152" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F152">
         <v>50</v>
       </c>
       <c r="G152" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="H152" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I152" t="s">
         <v>14</v>
@@ -4810,25 +4774,25 @@
     </row>
     <row r="153" spans="1:9">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B153" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D153">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="F153">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G153" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H153" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="I153" t="s">
         <v>14</v>
@@ -4836,25 +4800,25 @@
     </row>
     <row r="154" spans="1:9">
       <c r="A154" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B154" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D154">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E154" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F154">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G154" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H154" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="I154" t="s">
         <v>14</v>
@@ -4862,25 +4826,25 @@
     </row>
     <row r="155" spans="1:9">
       <c r="A155" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B155" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="D155">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E155" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F155">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G155" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H155" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I155" t="s">
         <v>14</v>
@@ -4888,25 +4852,25 @@
     </row>
     <row r="156" spans="1:9">
       <c r="A156" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D156">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E156" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="F156">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G156" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H156" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I156" t="s">
         <v>14</v>
@@ -4914,25 +4878,25 @@
     </row>
     <row r="157" spans="1:9">
       <c r="A157" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B157" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D157">
         <v>2</v>
       </c>
       <c r="E157" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="F157">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G157" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H157" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I157" t="s">
         <v>14</v>
@@ -4940,25 +4904,25 @@
     </row>
     <row r="158" spans="1:9">
       <c r="A158" t="s">
-        <v>128</v>
+        <v>47</v>
       </c>
       <c r="B158" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="D158">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E158" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F158">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G158" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H158" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I158" t="s">
         <v>14</v>
@@ -4966,28 +4930,25 @@
     </row>
     <row r="159" spans="1:9">
       <c r="A159" t="s">
-        <v>30</v>
+        <v>126</v>
       </c>
       <c r="B159" t="s">
-        <v>131</v>
-      </c>
-      <c r="C159" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="D159">
         <v>1</v>
       </c>
       <c r="E159" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="F159">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G159" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H159" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="I159" t="s">
         <v>14</v>
@@ -4995,25 +4956,25 @@
     </row>
     <row r="160" spans="1:9">
       <c r="A160" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B160" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D160">
         <v>1</v>
       </c>
       <c r="E160" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F160">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G160" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H160" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I160" t="s">
         <v>14</v>
@@ -5021,25 +4982,25 @@
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B161" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="D161">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E161" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F161">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G161" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H161" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I161" t="s">
         <v>14</v>
@@ -5047,25 +5008,25 @@
     </row>
     <row r="162" spans="1:9">
       <c r="A162" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="B162" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D162">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E162" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F162">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G162" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H162" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="I162" t="s">
         <v>14</v>
@@ -5073,328 +5034,28 @@
     </row>
     <row r="163" spans="1:9">
       <c r="A163" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="B163" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="D163">
         <v>1</v>
       </c>
       <c r="E163" t="s">
-        <v>130</v>
+        <v>37</v>
       </c>
       <c r="F163">
         <v>50</v>
       </c>
       <c r="G163" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="H163" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I163" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
-      <c r="A164" t="s">
-        <v>136</v>
-      </c>
-      <c r="B164" t="s">
-        <v>137</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-      <c r="E164" t="s">
-        <v>138</v>
-      </c>
-      <c r="F164">
-        <v>50</v>
-      </c>
-      <c r="G164" t="s">
-        <v>134</v>
-      </c>
-      <c r="H164" t="s">
-        <v>29</v>
-      </c>
-      <c r="I164" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9">
-      <c r="A165" t="s">
-        <v>67</v>
-      </c>
-      <c r="B165" t="s">
-        <v>68</v>
-      </c>
-      <c r="D165">
-        <v>2</v>
-      </c>
-      <c r="E165" t="s">
-        <v>83</v>
-      </c>
-      <c r="F165">
-        <v>40</v>
-      </c>
-      <c r="G165" t="s">
-        <v>139</v>
-      </c>
-      <c r="H165" t="s">
-        <v>43</v>
-      </c>
-      <c r="I165" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9">
-      <c r="A166" t="s">
-        <v>47</v>
-      </c>
-      <c r="B166" t="s">
-        <v>48</v>
-      </c>
-      <c r="D166">
-        <v>2</v>
-      </c>
-      <c r="E166" t="s">
-        <v>100</v>
-      </c>
-      <c r="F166">
-        <v>40</v>
-      </c>
-      <c r="G166" t="s">
-        <v>139</v>
-      </c>
-      <c r="H166" t="s">
-        <v>18</v>
-      </c>
-      <c r="I166" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9">
-      <c r="A167" t="s">
-        <v>125</v>
-      </c>
-      <c r="B167" t="s">
-        <v>126</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-      <c r="E167" t="s">
-        <v>21</v>
-      </c>
-      <c r="F167">
-        <v>40</v>
-      </c>
-      <c r="G167" t="s">
-        <v>139</v>
-      </c>
-      <c r="H167" t="s">
-        <v>22</v>
-      </c>
-      <c r="I167" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
-      <c r="A168" t="s">
-        <v>95</v>
-      </c>
-      <c r="B168" t="s">
-        <v>36</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168" t="s">
-        <v>112</v>
-      </c>
-      <c r="F168">
-        <v>40</v>
-      </c>
-      <c r="G168" t="s">
-        <v>139</v>
-      </c>
-      <c r="H168" t="s">
-        <v>23</v>
-      </c>
-      <c r="I168" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9">
-      <c r="A169" t="s">
-        <v>140</v>
-      </c>
-      <c r="B169" t="s">
-        <v>141</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-      <c r="E169" t="s">
-        <v>142</v>
-      </c>
-      <c r="F169">
-        <v>50</v>
-      </c>
-      <c r="G169" t="s">
-        <v>139</v>
-      </c>
-      <c r="H169" t="s">
-        <v>26</v>
-      </c>
-      <c r="I169" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
-      <c r="A170" t="s">
-        <v>143</v>
-      </c>
-      <c r="B170" t="s">
-        <v>25</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-      <c r="E170" t="s">
-        <v>110</v>
-      </c>
-      <c r="F170">
-        <v>50</v>
-      </c>
-      <c r="G170" t="s">
-        <v>139</v>
-      </c>
-      <c r="H170" t="s">
-        <v>29</v>
-      </c>
-      <c r="I170" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
-      <c r="A171" t="s">
-        <v>35</v>
-      </c>
-      <c r="B171" t="s">
-        <v>36</v>
-      </c>
-      <c r="D171">
-        <v>1</v>
-      </c>
-      <c r="E171" t="s">
-        <v>37</v>
-      </c>
-      <c r="F171">
-        <v>50</v>
-      </c>
-      <c r="G171" t="s">
-        <v>38</v>
-      </c>
-      <c r="H171" t="s">
-        <v>39</v>
-      </c>
-      <c r="I171" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
-      <c r="A172" t="s">
-        <v>144</v>
-      </c>
-      <c r="B172" t="s">
-        <v>145</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-      <c r="E172" t="s">
-        <v>21</v>
-      </c>
-      <c r="F172">
-        <v>50</v>
-      </c>
-      <c r="G172" t="s">
-        <v>99</v>
-      </c>
-      <c r="I172" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9">
-      <c r="A173" t="s">
-        <v>144</v>
-      </c>
-      <c r="B173" t="s">
-        <v>145</v>
-      </c>
-      <c r="D173">
-        <v>2</v>
-      </c>
-      <c r="E173" t="s">
-        <v>130</v>
-      </c>
-      <c r="F173">
-        <v>50</v>
-      </c>
-      <c r="G173" t="s">
-        <v>99</v>
-      </c>
-      <c r="I173" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9">
-      <c r="A174" t="s">
-        <v>59</v>
-      </c>
-      <c r="B174" t="s">
-        <v>60</v>
-      </c>
-      <c r="D174">
-        <v>2</v>
-      </c>
-      <c r="E174" t="s">
-        <v>21</v>
-      </c>
-      <c r="F174">
-        <v>40</v>
-      </c>
-      <c r="G174" t="s">
-        <v>99</v>
-      </c>
-      <c r="I174" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9">
-      <c r="A175" t="s">
-        <v>30</v>
-      </c>
-      <c r="B175" t="s">
-        <v>147</v>
-      </c>
-      <c r="D175">
-        <v>1</v>
-      </c>
-      <c r="E175" t="s">
-        <v>21</v>
-      </c>
-      <c r="F175">
-        <v>50</v>
-      </c>
-      <c r="G175" t="s">
-        <v>99</v>
-      </c>
-      <c r="I175" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -5404,69 +5065,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alternatives and schedules work working on multiple schedules and marron error and fixing output
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="155">
   <si>
     <t>Course</t>
   </si>
@@ -62,393 +62,390 @@
     <t>10:00:00</t>
   </si>
   <si>
+    <t>Public Policy 105</t>
+  </si>
+  <si>
+    <t>scheduled</t>
+  </si>
+  <si>
+    <t>CMSC 291</t>
+  </si>
+  <si>
+    <t>Continued Computer Science for Non-Majors</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Mon/Wed</t>
+  </si>
+  <si>
     <t>Information Technology 227</t>
   </si>
   <si>
-    <t>scheduled</t>
-  </si>
-  <si>
-    <t>CMSC  291</t>
-  </si>
-  <si>
-    <t>Continued Computer Science for Non-Majors</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>Mon/Wed</t>
+    <t>CMSC 341</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Marron, Christopher</t>
+  </si>
+  <si>
+    <t>Engineering 122, Engineering 122A</t>
+  </si>
+  <si>
+    <t>CMSC 441</t>
+  </si>
+  <si>
+    <t>Sherman Hall 013</t>
+  </si>
+  <si>
+    <t>CMSC 201</t>
+  </si>
+  <si>
+    <t>Computer Science I</t>
+  </si>
+  <si>
+    <t>Hamilton, Eric</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>CMSC 202</t>
+  </si>
+  <si>
+    <t>Computer Science II</t>
+  </si>
+  <si>
+    <t>Dixon, Jeremy</t>
+  </si>
+  <si>
+    <t>CMSC 203</t>
+  </si>
+  <si>
+    <t>Discrete Structures</t>
+  </si>
+  <si>
+    <t>Joeg, Prasanna</t>
+  </si>
+  <si>
+    <t>CMSC 313</t>
+  </si>
+  <si>
+    <t>Comp. Org. &amp; Assembly Lang.</t>
+  </si>
+  <si>
+    <t>Kartchner, Jeannette</t>
+  </si>
+  <si>
+    <t>CMSC 331</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Donyaee, Kash</t>
+  </si>
+  <si>
+    <t>Janet &amp; Walter Sondheim 109</t>
+  </si>
+  <si>
+    <t>Johnson, Benjamin</t>
+  </si>
+  <si>
+    <t>Math &amp; Psychology 106</t>
+  </si>
+  <si>
+    <t>CMSC 411cs</t>
+  </si>
+  <si>
+    <t>Computer Architecture</t>
+  </si>
+  <si>
+    <t>Sekyonda, Ivan</t>
+  </si>
+  <si>
+    <t>Meyerhoff Chemistry 030</t>
+  </si>
+  <si>
+    <t>CMSC 435/634</t>
+  </si>
+  <si>
+    <t>Computer Graphics</t>
+  </si>
+  <si>
+    <t>Olano, Marc</t>
+  </si>
+  <si>
+    <t>Sherman Hall 014</t>
+  </si>
+  <si>
+    <t>CMSC 447</t>
+  </si>
+  <si>
+    <t>Software Engineering I</t>
+  </si>
+  <si>
+    <t>Dutt, Abhijit</t>
   </si>
   <si>
     <t>Sherman Hall 151</t>
   </si>
   <si>
-    <t>CMSC 341</t>
-  </si>
-  <si>
-    <t>Data Structures</t>
-  </si>
-  <si>
-    <t>Marron, Christopher</t>
+    <t>CMSC 476/676</t>
+  </si>
+  <si>
+    <t>Information Retrieval</t>
+  </si>
+  <si>
+    <t>Pearce, Claudia</t>
+  </si>
+  <si>
+    <t>Interdisciplinary Life S 237</t>
+  </si>
+  <si>
+    <t>CMSC 201ss</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t>Bargteil, Adam</t>
+  </si>
+  <si>
+    <t>CMSC 461</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>CMSC 684</t>
+  </si>
+  <si>
+    <t>Wireless Sensor Networks</t>
+  </si>
+  <si>
+    <t>Younis, Mohamed</t>
   </si>
   <si>
     <t>Biological Sciences 120</t>
   </si>
   <si>
-    <t>CMSC 441</t>
-  </si>
-  <si>
-    <t>Interdisciplinary Life S 233</t>
-  </si>
-  <si>
-    <t>CMSC 201</t>
-  </si>
-  <si>
-    <t>Computer Science I</t>
-  </si>
-  <si>
-    <t>Hamilton, Eric</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>Public Policy 105</t>
-  </si>
-  <si>
-    <t>CMSC 202</t>
-  </si>
-  <si>
-    <t>Computer Science II</t>
-  </si>
-  <si>
-    <t>Dixon, Jeremy</t>
-  </si>
-  <si>
-    <t>Engineering 122, Engineering 122A</t>
-  </si>
-  <si>
-    <t>CMSC 203</t>
-  </si>
-  <si>
-    <t>Discrete Structures</t>
-  </si>
-  <si>
-    <t>Joeg, Prasanna</t>
-  </si>
-  <si>
-    <t>CMSC 313</t>
-  </si>
-  <si>
-    <t>Comp. Org. &amp; Assembly Lang.</t>
-  </si>
-  <si>
-    <t>Kartchner, Jeannette</t>
-  </si>
-  <si>
-    <t>CMSC 331</t>
-  </si>
-  <si>
-    <t>Programming Languages</t>
-  </si>
-  <si>
-    <t>Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>Math &amp; Psychology 106</t>
-  </si>
-  <si>
-    <t>Johnson, Benjamin</t>
-  </si>
-  <si>
-    <t>Sherman Hall 013</t>
-  </si>
-  <si>
-    <t>CMSC 411cs</t>
-  </si>
-  <si>
-    <t>Computer Architecture</t>
-  </si>
-  <si>
-    <t>Sekyonda, Ivan</t>
-  </si>
-  <si>
-    <t>Janet &amp; Walter Sondheim 109</t>
-  </si>
-  <si>
-    <t>CMSC 435/634</t>
-  </si>
-  <si>
-    <t>Computer Graphics</t>
-  </si>
-  <si>
-    <t>Olano, Marc</t>
-  </si>
-  <si>
-    <t>Meyerhoff Chemistry 030</t>
-  </si>
-  <si>
-    <t>CMSC 447</t>
-  </si>
-  <si>
-    <t>Software Engineering I</t>
-  </si>
-  <si>
-    <t>Dutt, Abhijit</t>
-  </si>
-  <si>
-    <t>CMSC 476/676</t>
-  </si>
-  <si>
-    <t>Information Retrieval</t>
-  </si>
-  <si>
-    <t>Pearce, Claudia</t>
-  </si>
-  <si>
-    <t>Sherman Hall 014</t>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>CMSC 455</t>
+  </si>
+  <si>
+    <t>Numerical Computations</t>
+  </si>
+  <si>
+    <t>Squire, Jon</t>
+  </si>
+  <si>
+    <t>CMSC 471</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Vafaei, Fereydoon</t>
+  </si>
+  <si>
+    <t>CMSC 491</t>
+  </si>
+  <si>
+    <t>Spec Topic: Data Science</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>CMSC 691</t>
+  </si>
+  <si>
+    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Ferraro, Frank</t>
+  </si>
+  <si>
+    <t>CMSC 104</t>
+  </si>
+  <si>
+    <t>Problem Solving &amp; Prog.</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>CMSC 304</t>
+  </si>
+  <si>
+    <t>Social &amp; Ethical Issues in IT</t>
+  </si>
+  <si>
+    <t>CMSC 421</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
   </si>
   <si>
     <t>CMSC 491/691</t>
   </si>
   <si>
+    <t>Spec Topic: Malware</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Nicholas, Charles</t>
+  </si>
+  <si>
+    <t>19:10:00</t>
+  </si>
+  <si>
+    <t>Tues/Thurs</t>
+  </si>
+  <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
+    <t>Chang, Richard</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>Kalpakis, Kostas</t>
+  </si>
+  <si>
+    <t>CMSC 478</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Wilson, Marcella</t>
+  </si>
+  <si>
+    <t>CMSC 426</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>CMSC 493</t>
+  </si>
+  <si>
+    <t>Games Capstone</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>CMSC 621</t>
+  </si>
+  <si>
+    <t>CMSC 411ce</t>
+  </si>
+  <si>
+    <t>Perkins, Dmitri</t>
+  </si>
+  <si>
+    <t>CMSC 479/679</t>
+  </si>
+  <si>
+    <t>Introduction to Robotics</t>
+  </si>
+  <si>
+    <t>Matuszek, Cynthia</t>
+  </si>
+  <si>
+    <t>CMSC 678</t>
+  </si>
+  <si>
+    <t>Oates, Tim</t>
+  </si>
+  <si>
+    <t>Finin, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 481</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>Spec Topic: Computer Vision</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Chapman, David</t>
+  </si>
+  <si>
+    <t>CMSC 611</t>
+  </si>
+  <si>
+    <t>Liu, Chenchen</t>
+  </si>
+  <si>
+    <t>CMSC 483/691</t>
+  </si>
+  <si>
+    <t>Parallel &amp; Distr. Processing</t>
+  </si>
+  <si>
+    <t>Simon, Tyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spec Topic: Quantum Security </t>
+  </si>
+  <si>
+    <t>CMSC 487/687</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Zieglar, Edward</t>
+  </si>
+  <si>
+    <t>unscheduled</t>
+  </si>
+  <si>
+    <t>CMSC 682</t>
+  </si>
+  <si>
+    <t>Network Technologies</t>
+  </si>
+  <si>
     <t>Spec Topic: Data Driven Design of Autonmous Systems</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
     <t>Zhu, Ting</t>
   </si>
   <si>
-    <t>CMSC 201ss</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t>Bargteil, Adam</t>
-  </si>
-  <si>
-    <t>CMSC 461</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>CMSC 684</t>
-  </si>
-  <si>
-    <t>Wireless Sensor Networks</t>
-  </si>
-  <si>
-    <t>Younis, Mohamed</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>CMSC 455</t>
-  </si>
-  <si>
-    <t>Numerical Computations</t>
-  </si>
-  <si>
-    <t>Squire, Jon</t>
-  </si>
-  <si>
-    <t>CMSC 471</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 491</t>
-  </si>
-  <si>
-    <t>Spec Topic: Data Science</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>CMSC 691</t>
-  </si>
-  <si>
-    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Ferraro, Frank</t>
-  </si>
-  <si>
-    <t>CMSC 104</t>
-  </si>
-  <si>
-    <t>Problem Solving &amp; Prog.</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>CMSC 304</t>
-  </si>
-  <si>
-    <t>Social &amp; Ethical Issues in IT</t>
-  </si>
-  <si>
-    <t>CMSC 421</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>Spec Topic: Malware</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Nicholas, Charles</t>
-  </si>
-  <si>
-    <t>19:10:00</t>
-  </si>
-  <si>
-    <t>Tues/Thurs</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>CMSC 478</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>CMSC 426</t>
-  </si>
-  <si>
-    <t>Computer Security</t>
-  </si>
-  <si>
-    <t>CMSC 493</t>
-  </si>
-  <si>
-    <t>Games Capstone</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>CMSC 621</t>
-  </si>
-  <si>
-    <t>CMSC 411ce</t>
-  </si>
-  <si>
-    <t>Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 479/679</t>
-  </si>
-  <si>
-    <t>Introduction to Robotics</t>
-  </si>
-  <si>
-    <t>Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 678</t>
-  </si>
-  <si>
-    <t>Oates, Tim</t>
-  </si>
-  <si>
-    <t>Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 481</t>
-  </si>
-  <si>
-    <t>Computer Networks</t>
-  </si>
-  <si>
-    <t>Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>Spec Topic: Computer Vision</t>
-  </si>
-  <si>
-    <t>Chapman, David</t>
-  </si>
-  <si>
-    <t>CMSC 611</t>
-  </si>
-  <si>
-    <t>Liu, Chenchen</t>
-  </si>
-  <si>
-    <t>CMSC 483/691</t>
-  </si>
-  <si>
-    <t>Parallel &amp; Distr. Processing</t>
-  </si>
-  <si>
-    <t>Simon, Tyler</t>
-  </si>
-  <si>
-    <t>Interdisciplinary Life S 237</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spec Topic: Quantum Security </t>
-  </si>
-  <si>
-    <t>CMSC 487/687</t>
-  </si>
-  <si>
-    <t>Network Security</t>
-  </si>
-  <si>
-    <t>Zieglar, Edward</t>
-  </si>
-  <si>
-    <t>CMSC 682</t>
-  </si>
-  <si>
-    <t>Network Technologies</t>
-  </si>
-  <si>
-    <t>unscheduled</t>
-  </si>
-  <si>
     <t>course</t>
   </si>
   <si>
@@ -461,19 +458,25 @@
     <t>alt3</t>
   </si>
   <si>
+    <t>CMSC 611Computer Architecture2Staff</t>
+  </si>
+  <si>
+    <t>{'mw230': Sherman Hall 014}</t>
+  </si>
+  <si>
+    <t>{'mw230': Interdisciplinary Life S 237}</t>
+  </si>
+  <si>
+    <t>{'mw230': Public Policy 105}</t>
+  </si>
+  <si>
+    <t>CMSC 682Network Technologies1Staff</t>
+  </si>
+  <si>
     <t>CMSC 682Network Technologies2Sidhu, Deepinder</t>
   </si>
   <si>
-    <t>{'mw530': Interdisciplinary Life S 237}</t>
-  </si>
-  <si>
-    <t>{'mw530': Public Policy 105}</t>
-  </si>
-  <si>
-    <t>{'mw230': Sherman Hall 014}</t>
-  </si>
-  <si>
-    <t>CMSC 684Wireless Sensor Networks2Staff</t>
+    <t>CMSC 491/691Spec Topic: Data Driven Design of Autonmous Systems1Zhu, Ting</t>
   </si>
   <si>
     <t>CMSC 491/691Spec Topic: Internet of Things 1Staff</t>
@@ -985,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -993,16 +996,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -1014,7 +1017,7 @@
         <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -1022,16 +1025,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>40</v>
@@ -1043,7 +1046,7 @@
         <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -1051,16 +1054,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>40</v>
@@ -1080,16 +1083,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -1101,7 +1104,7 @@
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
@@ -1118,7 +1121,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -1130,7 +1133,7 @@
         <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1138,16 +1141,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
       </c>
       <c r="F12">
         <v>40</v>
@@ -1159,7 +1162,7 @@
         <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
@@ -1167,16 +1170,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
       </c>
       <c r="F13">
         <v>50</v>
@@ -1188,7 +1191,7 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
@@ -1196,16 +1199,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>57</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
       </c>
       <c r="F14">
         <v>30</v>
@@ -1217,7 +1220,7 @@
         <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="J14" t="s">
         <v>16</v>
@@ -1225,16 +1228,16 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>61</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
       </c>
       <c r="F15">
         <v>50</v>
@@ -1246,7 +1249,7 @@
         <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J15" t="s">
         <v>16</v>
@@ -1254,31 +1257,28 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" t="s">
-        <v>31</v>
-      </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
         <v>16</v>
@@ -1286,28 +1286,28 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F17">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J17" t="s">
         <v>16</v>
@@ -1315,16 +1315,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F18">
         <v>40</v>
@@ -1333,10 +1333,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
@@ -1344,16 +1344,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F19">
         <v>40</v>
@@ -1362,10 +1362,10 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I19" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -1373,16 +1373,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>40</v>
@@ -1391,7 +1391,7 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
@@ -1402,28 +1402,28 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F21">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J21" t="s">
         <v>16</v>
@@ -1431,28 +1431,28 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="F22">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="J22" t="s">
         <v>16</v>
@@ -1460,28 +1460,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" t="s">
-        <v>52</v>
       </c>
       <c r="J23" t="s">
         <v>16</v>
@@ -1489,28 +1489,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="F24">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -1518,28 +1518,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I25" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J25" t="s">
         <v>16</v>
@@ -1547,16 +1547,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="F26">
         <v>40</v>
@@ -1565,10 +1565,10 @@
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J26" t="s">
         <v>16</v>
@@ -1576,28 +1576,28 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>78</v>
       </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
       <c r="F27">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I27" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="J27" t="s">
         <v>16</v>
@@ -1605,28 +1605,31 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F28">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J28" t="s">
         <v>16</v>
@@ -1634,31 +1637,31 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>85</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
       <c r="F29">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -1671,26 +1674,23 @@
       <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30">
+        <v>40</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
         <v>88</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30">
-        <v>50</v>
-      </c>
-      <c r="G30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" t="s">
-        <v>76</v>
-      </c>
       <c r="I30" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="J30" t="s">
         <v>16</v>
@@ -1698,25 +1698,25 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F31">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s">
         <v>25</v>
@@ -1727,28 +1727,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J32" t="s">
         <v>16</v>
@@ -1756,16 +1756,16 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F33">
         <v>40</v>
@@ -1774,10 +1774,10 @@
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J33" t="s">
         <v>16</v>
@@ -1785,13 +1785,13 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -1803,7 +1803,7 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
         <v>46</v>
@@ -1814,13 +1814,13 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -1832,10 +1832,10 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J35" t="s">
         <v>16</v>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1855,16 +1855,16 @@
         <v>19</v>
       </c>
       <c r="F36">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s">
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I36" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -1872,16 +1872,19 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F37">
         <v>50</v>
@@ -1890,10 +1893,10 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I37" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="J37" t="s">
         <v>16</v>
@@ -1901,31 +1904,28 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
         <v>97</v>
       </c>
-      <c r="C38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38">
-        <v>50</v>
-      </c>
-      <c r="G38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" t="s">
-        <v>92</v>
-      </c>
       <c r="I38" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s">
         <v>16</v>
@@ -1933,25 +1933,25 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="H39" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="I39" t="s">
         <v>25</v>
@@ -1962,28 +1962,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="F40">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J40" t="s">
         <v>16</v>
@@ -1991,28 +1991,28 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="F41">
         <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H41" t="s">
         <v>14</v>
       </c>
       <c r="I41" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J41" t="s">
         <v>16</v>
@@ -2020,28 +2020,28 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F42">
         <v>40</v>
       </c>
       <c r="G42" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J42" t="s">
         <v>16</v>
@@ -2049,28 +2049,28 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
         <v>103</v>
       </c>
       <c r="F43">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H43" t="s">
         <v>14</v>
       </c>
       <c r="I43" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J43" t="s">
         <v>16</v>
@@ -2078,28 +2078,28 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+      <c r="G44" t="s">
+        <v>98</v>
+      </c>
+      <c r="H44" t="s">
         <v>104</v>
       </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44">
-        <v>50</v>
-      </c>
-      <c r="G44" t="s">
-        <v>101</v>
-      </c>
-      <c r="H44" t="s">
-        <v>14</v>
-      </c>
       <c r="I44" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="J44" t="s">
         <v>16</v>
@@ -2107,28 +2107,28 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="F45">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I45" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J45" t="s">
         <v>16</v>
@@ -2136,28 +2136,28 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="F46">
         <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H46" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I46" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J46" t="s">
         <v>16</v>
@@ -2165,28 +2165,28 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="F47">
         <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I47" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J47" t="s">
         <v>16</v>
@@ -2194,25 +2194,25 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="F48">
         <v>40</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I48" t="s">
         <v>46</v>
@@ -2223,28 +2223,28 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="F49">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G49" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H49" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I49" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J49" t="s">
         <v>16</v>
@@ -2252,28 +2252,28 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F50">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G50" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H50" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="I50" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="J50" t="s">
         <v>16</v>
@@ -2281,22 +2281,22 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="F51">
         <v>40</v>
       </c>
       <c r="G51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H51" t="s">
         <v>31</v>
@@ -2310,22 +2310,22 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F52">
         <v>40</v>
       </c>
       <c r="G52" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H52" t="s">
         <v>31</v>
@@ -2339,28 +2339,28 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F53">
         <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H53" t="s">
         <v>31</v>
       </c>
       <c r="I53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J53" t="s">
         <v>16</v>
@@ -2368,28 +2368,28 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F54">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H54" t="s">
         <v>31</v>
       </c>
       <c r="I54" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J54" t="s">
         <v>16</v>
@@ -2400,25 +2400,25 @@
         <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F55">
         <v>50</v>
       </c>
       <c r="G55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H55" t="s">
         <v>31</v>
       </c>
       <c r="I55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J55" t="s">
         <v>16</v>
@@ -2426,28 +2426,28 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="F56">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G56" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H56" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="I56" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="J56" t="s">
         <v>16</v>
@@ -2455,28 +2455,28 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D57">
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="F57">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H57" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I57" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J57" t="s">
         <v>16</v>
@@ -2484,28 +2484,28 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="F58">
         <v>40</v>
       </c>
       <c r="G58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H58" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I58" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J58" t="s">
         <v>16</v>
@@ -2513,28 +2513,28 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="F59">
         <v>40</v>
       </c>
       <c r="G59" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H59" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I59" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="J59" t="s">
         <v>16</v>
@@ -2542,28 +2542,28 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>119</v>
       </c>
       <c r="F60">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G60" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H60" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I60" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J60" t="s">
         <v>16</v>
@@ -2574,25 +2574,25 @@
         <v>120</v>
       </c>
       <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>121</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>122</v>
       </c>
       <c r="F61">
         <v>50</v>
       </c>
       <c r="G61" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H61" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="I61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J61" t="s">
         <v>16</v>
@@ -2600,28 +2600,28 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="F62">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I62" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="J62" t="s">
         <v>16</v>
@@ -2629,28 +2629,28 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F63">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G63" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H63" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I63" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J63" t="s">
         <v>16</v>
@@ -2658,28 +2658,28 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="F64">
         <v>40</v>
       </c>
       <c r="G64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H64" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I64" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J64" t="s">
         <v>16</v>
@@ -2687,28 +2687,28 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65">
+        <v>40</v>
+      </c>
+      <c r="G65" t="s">
+        <v>98</v>
+      </c>
+      <c r="H65" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" t="s">
         <v>44</v>
-      </c>
-      <c r="D65">
-        <v>4</v>
-      </c>
-      <c r="E65" t="s">
-        <v>82</v>
-      </c>
-      <c r="F65">
-        <v>40</v>
-      </c>
-      <c r="G65" t="s">
-        <v>101</v>
-      </c>
-      <c r="H65" t="s">
-        <v>76</v>
-      </c>
-      <c r="I65" t="s">
-        <v>27</v>
       </c>
       <c r="J65" t="s">
         <v>16</v>
@@ -2716,28 +2716,28 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="F66">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G66" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I66" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J66" t="s">
         <v>16</v>
@@ -2745,13 +2745,13 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" t="s">
         <v>125</v>
@@ -2760,13 +2760,13 @@
         <v>50</v>
       </c>
       <c r="G67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H67" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J67" t="s">
         <v>16</v>
@@ -2774,9 +2774,12 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" t="s">
         <v>126</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>127</v>
       </c>
       <c r="D68">
@@ -2789,13 +2792,13 @@
         <v>50</v>
       </c>
       <c r="G68" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H68" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I68" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="J68" t="s">
         <v>16</v>
@@ -2803,13 +2806,10 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
-      </c>
-      <c r="C69" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2821,13 +2821,13 @@
         <v>50</v>
       </c>
       <c r="G69" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H69" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I69" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="J69" t="s">
         <v>16</v>
@@ -2835,28 +2835,28 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>132</v>
+        <v>19</v>
       </c>
       <c r="F70">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G70" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H70" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="I70" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J70" t="s">
         <v>16</v>
@@ -2864,13 +2864,13 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
@@ -2879,10 +2879,10 @@
         <v>40</v>
       </c>
       <c r="G71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H71" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I71" t="s">
         <v>25</v>
@@ -2893,28 +2893,28 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="F72">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G72" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H72" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I72" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="J72" t="s">
         <v>16</v>
@@ -2922,28 +2922,28 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F73">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G73" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H73" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I73" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J73" t="s">
         <v>16</v>
@@ -2951,10 +2951,10 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -2963,16 +2963,16 @@
         <v>19</v>
       </c>
       <c r="F74">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G74" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H74" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I74" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="J74" t="s">
         <v>16</v>
@@ -2980,13 +2980,13 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
@@ -2995,10 +2995,10 @@
         <v>40</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H75" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I75" t="s">
         <v>46</v>
@@ -3009,13 +3009,13 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
         <v>19</v>
@@ -3024,13 +3024,13 @@
         <v>40</v>
       </c>
       <c r="G76" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H76" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I76" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J76" t="s">
         <v>16</v>
@@ -3038,28 +3038,28 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="D77">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E77" t="s">
         <v>19</v>
       </c>
       <c r="F77">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H77" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I77" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="J77" t="s">
         <v>16</v>
@@ -3067,28 +3067,28 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
       </c>
       <c r="F78">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G78" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H78" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I78" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J78" t="s">
         <v>16</v>
@@ -3096,28 +3096,28 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="F79">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G79" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H79" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I79" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="J79" t="s">
         <v>16</v>
@@ -3125,28 +3125,28 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
       </c>
       <c r="F80">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H80" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I80" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J80" t="s">
         <v>16</v>
@@ -3154,28 +3154,28 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="F81">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H81" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I81" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J81" t="s">
         <v>16</v>
@@ -3183,28 +3183,28 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G82" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H82" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I82" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="J82" t="s">
         <v>16</v>
@@ -3212,28 +3212,28 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="F83">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H83" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I83" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="J83" t="s">
         <v>16</v>
@@ -3241,28 +3241,28 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="B84" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="D84">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="F84">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G84" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H84" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I84" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="J84" t="s">
         <v>16</v>
@@ -3270,68 +3270,50 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="F85">
-        <v>50</v>
-      </c>
-      <c r="G85" t="s">
-        <v>101</v>
-      </c>
-      <c r="H85" t="s">
-        <v>100</v>
-      </c>
-      <c r="I85" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="J85" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="F86">
         <v>50</v>
       </c>
-      <c r="G86" t="s">
-        <v>101</v>
-      </c>
-      <c r="H86" t="s">
-        <v>100</v>
-      </c>
-      <c r="I86" t="s">
-        <v>56</v>
-      </c>
       <c r="J86" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B87" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -3343,47 +3325,50 @@
         <v>50</v>
       </c>
       <c r="J87" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B88" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D88">
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F88">
         <v>50</v>
       </c>
       <c r="J88" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>74</v>
+        <v>141</v>
+      </c>
+      <c r="C89" t="s">
+        <v>127</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="F89">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J89" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3393,7 +3378,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3401,58 +3386,86 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
         <v>144</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>146</v>
-      </c>
-      <c r="D1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
         <v>148</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>150</v>
-      </c>
-      <c r="D2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
         <v>149</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>150</v>
-      </c>
-      <c r="D3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>153</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
         <v>149</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>150</v>
       </c>
-      <c r="D4" t="s">
-        <v>151</v>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple schedules made working on minor bug fixes
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="157">
   <si>
     <t>Course</t>
   </si>
@@ -62,75 +62,114 @@
     <t>10:00:00</t>
   </si>
   <si>
+    <t>Janet &amp; Walter Sondheim 109</t>
+  </si>
+  <si>
+    <t>scheduled</t>
+  </si>
+  <si>
+    <t>CMSC 341</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Marron, Christopher</t>
+  </si>
+  <si>
+    <t>Mon/Wed</t>
+  </si>
+  <si>
+    <t>Information Technology 227</t>
+  </si>
+  <si>
+    <t>CMSC 441</t>
+  </si>
+  <si>
+    <t>Engineering 122, Engineering 122A</t>
+  </si>
+  <si>
+    <t>CMSC 291</t>
+  </si>
+  <si>
+    <t>Continued Computer Science for Non-Majors</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Sherman Hall 151</t>
+  </si>
+  <si>
+    <t>CMSC 201</t>
+  </si>
+  <si>
+    <t>Computer Science I</t>
+  </si>
+  <si>
+    <t>Hamilton, Eric</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
     <t>Public Policy 105</t>
   </si>
   <si>
-    <t>scheduled</t>
-  </si>
-  <si>
-    <t>CMSC 291</t>
-  </si>
-  <si>
-    <t>Continued Computer Science for Non-Majors</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>Mon/Wed</t>
-  </si>
-  <si>
-    <t>Information Technology 227</t>
-  </si>
-  <si>
-    <t>CMSC 341</t>
-  </si>
-  <si>
-    <t>Data Structures</t>
-  </si>
-  <si>
-    <t>Marron, Christopher</t>
-  </si>
-  <si>
-    <t>Engineering 122, Engineering 122A</t>
-  </si>
-  <si>
-    <t>CMSC 441</t>
+    <t>CMSC 202</t>
+  </si>
+  <si>
+    <t>Computer Science II</t>
+  </si>
+  <si>
+    <t>Dixon, Jeremy</t>
+  </si>
+  <si>
+    <t>CMSC 435/634</t>
+  </si>
+  <si>
+    <t>Computer Graphics</t>
+  </si>
+  <si>
+    <t>Olano, Marc</t>
+  </si>
+  <si>
+    <t>CMSC 476/676</t>
+  </si>
+  <si>
+    <t>Information Retrieval</t>
+  </si>
+  <si>
+    <t>Pearce, Claudia</t>
+  </si>
+  <si>
+    <t>Sherman Hall 014</t>
+  </si>
+  <si>
+    <t>CMSC 491/691</t>
+  </si>
+  <si>
+    <t>Spec Topic: Data Driven Design of Autonmous Systems</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Zhu, Ting</t>
+  </si>
+  <si>
+    <t>CMSC 203</t>
+  </si>
+  <si>
+    <t>Discrete Structures</t>
+  </si>
+  <si>
+    <t>Joeg, Prasanna</t>
   </si>
   <si>
     <t>Sherman Hall 013</t>
   </si>
   <si>
-    <t>CMSC 201</t>
-  </si>
-  <si>
-    <t>Computer Science I</t>
-  </si>
-  <si>
-    <t>Hamilton, Eric</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>CMSC 202</t>
-  </si>
-  <si>
-    <t>Computer Science II</t>
-  </si>
-  <si>
-    <t>Dixon, Jeremy</t>
-  </si>
-  <si>
-    <t>CMSC 203</t>
-  </si>
-  <si>
-    <t>Discrete Structures</t>
-  </si>
-  <si>
-    <t>Joeg, Prasanna</t>
-  </si>
-  <si>
     <t>CMSC 313</t>
   </si>
   <si>
@@ -140,6 +179,9 @@
     <t>Kartchner, Jeannette</t>
   </si>
   <si>
+    <t>Math &amp; Psychology 106</t>
+  </si>
+  <si>
     <t>CMSC 331</t>
   </si>
   <si>
@@ -149,13 +191,13 @@
     <t>Donyaee, Kash</t>
   </si>
   <si>
-    <t>Janet &amp; Walter Sondheim 109</t>
+    <t>Meyerhoff Chemistry 030</t>
   </si>
   <si>
     <t>Johnson, Benjamin</t>
   </si>
   <si>
-    <t>Math &amp; Psychology 106</t>
+    <t>Biological Sciences 120</t>
   </si>
   <si>
     <t>CMSC 411cs</t>
@@ -167,19 +209,7 @@
     <t>Sekyonda, Ivan</t>
   </si>
   <si>
-    <t>Meyerhoff Chemistry 030</t>
-  </si>
-  <si>
-    <t>CMSC 435/634</t>
-  </si>
-  <si>
-    <t>Computer Graphics</t>
-  </si>
-  <si>
-    <t>Olano, Marc</t>
-  </si>
-  <si>
-    <t>Sherman Hall 014</t>
+    <t>Interdisciplinary Life S 233</t>
   </si>
   <si>
     <t>CMSC 447</t>
@@ -191,234 +221,219 @@
     <t>Dutt, Abhijit</t>
   </si>
   <si>
-    <t>Sherman Hall 151</t>
-  </si>
-  <si>
-    <t>CMSC 476/676</t>
-  </si>
-  <si>
-    <t>Information Retrieval</t>
-  </si>
-  <si>
-    <t>Pearce, Claudia</t>
+    <t>CMSC 201ss</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t>Bargteil, Adam</t>
+  </si>
+  <si>
+    <t>CMSC 461</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>CMSC 684</t>
+  </si>
+  <si>
+    <t>Wireless Sensor Networks</t>
+  </si>
+  <si>
+    <t>Younis, Mohamed</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>CMSC 471</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Vafaei, Fereydoon</t>
+  </si>
+  <si>
+    <t>CMSC 691</t>
+  </si>
+  <si>
+    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Ferraro, Frank</t>
+  </si>
+  <si>
+    <t>CMSC 455</t>
+  </si>
+  <si>
+    <t>Numerical Computations</t>
+  </si>
+  <si>
+    <t>Squire, Jon</t>
+  </si>
+  <si>
+    <t>CMSC 491</t>
+  </si>
+  <si>
+    <t>Spec Topic: Data Science</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>Spec Topic: Malware</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Nicholas, Charles</t>
+  </si>
+  <si>
+    <t>CMSC 104</t>
+  </si>
+  <si>
+    <t>Problem Solving &amp; Prog.</t>
+  </si>
+  <si>
+    <t>CMSC 304</t>
+  </si>
+  <si>
+    <t>Social &amp; Ethical Issues in IT</t>
+  </si>
+  <si>
+    <t>CMSC 421</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>19:10:00</t>
+  </si>
+  <si>
+    <t>Tues/Thurs</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
+    <t>Chang, Richard</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>CMSC 478</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Kalpakis, Kostas</t>
+  </si>
+  <si>
+    <t>CMSC 493</t>
+  </si>
+  <si>
+    <t>Games Capstone</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>CMSC 621</t>
+  </si>
+  <si>
+    <t>Wilson, Marcella</t>
+  </si>
+  <si>
+    <t>CMSC 426</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>CMSC 479/679</t>
+  </si>
+  <si>
+    <t>Introduction to Robotics</t>
+  </si>
+  <si>
+    <t>Matuszek, Cynthia</t>
+  </si>
+  <si>
+    <t>CMSC 678</t>
+  </si>
+  <si>
+    <t>Oates, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 411ce</t>
+  </si>
+  <si>
+    <t>Perkins, Dmitri</t>
+  </si>
+  <si>
+    <t>Finin, Tim</t>
+  </si>
+  <si>
+    <t>CMSC 481</t>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+  </si>
+  <si>
+    <t>Sidhu, Deepinder</t>
+  </si>
+  <si>
+    <t>Spec Topic: Computer Vision</t>
+  </si>
+  <si>
+    <t>Chapman, David</t>
+  </si>
+  <si>
+    <t>CMSC 611</t>
+  </si>
+  <si>
+    <t>Liu, Chenchen</t>
+  </si>
+  <si>
+    <t>CMSC 483/691</t>
+  </si>
+  <si>
+    <t>Parallel &amp; Distr. Processing</t>
+  </si>
+  <si>
+    <t>Simon, Tyler</t>
+  </si>
+  <si>
+    <t>CMSC 682</t>
+  </si>
+  <si>
+    <t>Network Technologies</t>
   </si>
   <si>
     <t>Interdisciplinary Life S 237</t>
   </si>
   <si>
-    <t>CMSC 201ss</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t>Bargteil, Adam</t>
-  </si>
-  <si>
-    <t>CMSC 461</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>CMSC 684</t>
-  </si>
-  <si>
-    <t>Wireless Sensor Networks</t>
-  </si>
-  <si>
-    <t>Younis, Mohamed</t>
-  </si>
-  <si>
-    <t>Biological Sciences 120</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>CMSC 455</t>
-  </si>
-  <si>
-    <t>Numerical Computations</t>
-  </si>
-  <si>
-    <t>Squire, Jon</t>
-  </si>
-  <si>
-    <t>CMSC 471</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 491</t>
-  </si>
-  <si>
-    <t>Spec Topic: Data Science</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>CMSC 691</t>
-  </si>
-  <si>
-    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Ferraro, Frank</t>
-  </si>
-  <si>
-    <t>CMSC 104</t>
-  </si>
-  <si>
-    <t>Problem Solving &amp; Prog.</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>CMSC 304</t>
-  </si>
-  <si>
-    <t>Social &amp; Ethical Issues in IT</t>
-  </si>
-  <si>
-    <t>CMSC 421</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>CMSC 491/691</t>
-  </si>
-  <si>
-    <t>Spec Topic: Malware</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Nicholas, Charles</t>
-  </si>
-  <si>
-    <t>19:10:00</t>
-  </si>
-  <si>
-    <t>Tues/Thurs</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
-    <t>Chang, Richard</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>Kalpakis, Kostas</t>
-  </si>
-  <si>
-    <t>CMSC 478</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Wilson, Marcella</t>
-  </si>
-  <si>
-    <t>CMSC 426</t>
-  </si>
-  <si>
-    <t>Computer Security</t>
-  </si>
-  <si>
-    <t>CMSC 493</t>
-  </si>
-  <si>
-    <t>Games Capstone</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>CMSC 621</t>
-  </si>
-  <si>
-    <t>CMSC 411ce</t>
-  </si>
-  <si>
-    <t>Perkins, Dmitri</t>
-  </si>
-  <si>
-    <t>CMSC 479/679</t>
-  </si>
-  <si>
-    <t>Introduction to Robotics</t>
-  </si>
-  <si>
-    <t>Matuszek, Cynthia</t>
-  </si>
-  <si>
-    <t>CMSC 678</t>
-  </si>
-  <si>
-    <t>Oates, Tim</t>
-  </si>
-  <si>
-    <t>Finin, Tim</t>
-  </si>
-  <si>
-    <t>CMSC 481</t>
-  </si>
-  <si>
-    <t>Computer Networks</t>
-  </si>
-  <si>
-    <t>Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>Spec Topic: Computer Vision</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Chapman, David</t>
-  </si>
-  <si>
-    <t>CMSC 611</t>
-  </si>
-  <si>
-    <t>Liu, Chenchen</t>
-  </si>
-  <si>
-    <t>CMSC 483/691</t>
-  </si>
-  <si>
-    <t>Parallel &amp; Distr. Processing</t>
-  </si>
-  <si>
-    <t>Simon, Tyler</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spec Topic: Quantum Security </t>
   </si>
   <si>
@@ -431,21 +446,12 @@
     <t>Zieglar, Edward</t>
   </si>
   <si>
+    <t xml:space="preserve">Spec Topic: Internet of Things </t>
+  </si>
+  <si>
     <t>unscheduled</t>
   </si>
   <si>
-    <t>CMSC 682</t>
-  </si>
-  <si>
-    <t>Network Technologies</t>
-  </si>
-  <si>
-    <t>Spec Topic: Data Driven Design of Autonmous Systems</t>
-  </si>
-  <si>
-    <t>Zhu, Ting</t>
-  </si>
-  <si>
     <t>course</t>
   </si>
   <si>
@@ -458,28 +464,28 @@
     <t>alt3</t>
   </si>
   <si>
-    <t>CMSC 611Computer Architecture2Staff</t>
+    <t>CMSC 491/691 Spec Topic: Internet of Things  1 Staff</t>
+  </si>
+  <si>
+    <t>{'mw530': Interdisciplinary Life S 237}</t>
+  </si>
+  <si>
+    <t>{'mw530': Public Policy 105}</t>
   </si>
   <si>
     <t>{'mw230': Sherman Hall 014}</t>
   </si>
   <si>
-    <t>{'mw230': Interdisciplinary Life S 237}</t>
-  </si>
-  <si>
-    <t>{'mw230': Public Policy 105}</t>
-  </si>
-  <si>
-    <t>CMSC 682Network Technologies1Staff</t>
-  </si>
-  <si>
-    <t>CMSC 682Network Technologies2Sidhu, Deepinder</t>
-  </si>
-  <si>
-    <t>CMSC 491/691Spec Topic: Data Driven Design of Autonmous Systems1Zhu, Ting</t>
-  </si>
-  <si>
-    <t>CMSC 491/691Spec Topic: Internet of Things 1Staff</t>
+    <t>CMSC 304 Social &amp; Ethical Issues in IT 6 Staff</t>
+  </si>
+  <si>
+    <t>{'mw230': Interdisciplinary Life S 233}</t>
+  </si>
+  <si>
+    <t>CMSC 411cs Computer Architecture 3 Staff</t>
+  </si>
+  <si>
+    <t>CMSC 684 Wireless Sensor Networks 2 Staff</t>
   </si>
 </sst>
 </file>
@@ -811,7 +817,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -892,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
@@ -912,13 +918,13 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>40</v>
@@ -930,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -938,19 +944,19 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
       <c r="F5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -988,7 +994,7 @@
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -996,16 +1002,16 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -1017,7 +1023,7 @@
         <v>31</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -1025,19 +1031,19 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
@@ -1054,19 +1060,19 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -1075,7 +1081,7 @@
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
@@ -1083,19 +1089,22 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F10">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -1104,7 +1113,7 @@
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
@@ -1112,16 +1121,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -1133,7 +1142,7 @@
         <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1141,16 +1150,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F12">
         <v>40</v>
@@ -1162,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
@@ -1170,19 +1179,19 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F13">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1191,7 +1200,7 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
@@ -1199,19 +1208,19 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -1220,7 +1229,7 @@
         <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
         <v>16</v>
@@ -1228,19 +1237,19 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F15">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1249,7 +1258,7 @@
         <v>31</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
         <v>16</v>
@@ -1257,28 +1266,28 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J16" t="s">
         <v>16</v>
@@ -1286,28 +1295,28 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F17">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
         <v>16</v>
@@ -1315,13 +1324,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>49</v>
@@ -1333,10 +1342,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
@@ -1344,16 +1353,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19">
         <v>40</v>
@@ -1362,10 +1371,10 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -1373,16 +1382,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="F20">
         <v>40</v>
@@ -1391,10 +1400,10 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="J20" t="s">
         <v>16</v>
@@ -1402,28 +1411,28 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F21">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J21" t="s">
         <v>16</v>
@@ -1431,16 +1440,16 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F22">
         <v>40</v>
@@ -1449,10 +1458,10 @@
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J22" t="s">
         <v>16</v>
@@ -1460,28 +1469,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
         <v>69</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" t="s">
-        <v>64</v>
-      </c>
       <c r="I23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
         <v>16</v>
@@ -1489,28 +1498,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24">
         <v>30</v>
       </c>
-      <c r="F24">
-        <v>100</v>
-      </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -1518,28 +1527,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" t="s">
         <v>23</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25">
-        <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" t="s">
-        <v>21</v>
       </c>
       <c r="J25" t="s">
         <v>16</v>
@@ -1547,28 +1556,28 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J26" t="s">
         <v>16</v>
@@ -1576,28 +1585,31 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27">
-        <v>50</v>
-      </c>
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" t="s">
-        <v>72</v>
-      </c>
       <c r="I27" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="J27" t="s">
         <v>16</v>
@@ -1605,19 +1617,16 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F28">
         <v>40</v>
@@ -1626,10 +1635,10 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J28" t="s">
         <v>16</v>
@@ -1637,31 +1646,28 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F29">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -1669,16 +1675,19 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F30">
         <v>40</v>
@@ -1687,10 +1696,10 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="J30" t="s">
         <v>16</v>
@@ -1698,16 +1707,16 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F31">
         <v>100</v>
@@ -1716,10 +1725,10 @@
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
@@ -1727,28 +1736,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F32">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I32" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
         <v>16</v>
@@ -1756,28 +1765,31 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" t="s">
         <v>90</v>
       </c>
-      <c r="D33">
-        <v>4</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33">
-        <v>40</v>
-      </c>
-      <c r="G33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" t="s">
-        <v>88</v>
-      </c>
       <c r="I33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J33" t="s">
         <v>16</v>
@@ -1785,28 +1797,28 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
         <v>90</v>
       </c>
-      <c r="D34">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34">
-        <v>40</v>
-      </c>
-      <c r="G34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" t="s">
-        <v>88</v>
-      </c>
       <c r="I34" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J34" t="s">
         <v>16</v>
@@ -1814,16 +1826,16 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F35">
         <v>40</v>
@@ -1832,10 +1844,10 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J35" t="s">
         <v>16</v>
@@ -1843,28 +1855,28 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F36">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G36" t="s">
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I36" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J36" t="s">
         <v>16</v>
@@ -1872,31 +1884,28 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="F37">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J37" t="s">
         <v>16</v>
@@ -1904,28 +1913,28 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
         <v>90</v>
       </c>
-      <c r="D38">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38">
-        <v>40</v>
-      </c>
-      <c r="G38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" t="s">
-        <v>97</v>
-      </c>
       <c r="I38" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="J38" t="s">
         <v>16</v>
@@ -1933,28 +1942,28 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F39">
+        <v>40</v>
+      </c>
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
         <v>100</v>
       </c>
-      <c r="G39" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" t="s">
-        <v>14</v>
-      </c>
       <c r="I39" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J39" t="s">
         <v>16</v>
@@ -1962,28 +1971,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>35</v>
       </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40" t="s">
-        <v>99</v>
-      </c>
       <c r="F40">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G40" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J40" t="s">
         <v>16</v>
@@ -1991,28 +2000,28 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="F41">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G41" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H41" t="s">
         <v>14</v>
       </c>
       <c r="I41" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J41" t="s">
         <v>16</v>
@@ -2020,28 +2029,28 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F42">
         <v>40</v>
       </c>
       <c r="G42" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J42" t="s">
         <v>16</v>
@@ -2049,28 +2058,28 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="F43">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H43" t="s">
         <v>14</v>
       </c>
       <c r="I43" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="J43" t="s">
         <v>16</v>
@@ -2078,28 +2087,28 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="F44">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G44" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H44" t="s">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="I44" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="J44" t="s">
         <v>16</v>
@@ -2107,28 +2116,28 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="F45">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H45" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J45" t="s">
         <v>16</v>
@@ -2136,28 +2145,28 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="F46">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G46" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H46" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I46" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J46" t="s">
         <v>16</v>
@@ -2165,28 +2174,28 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="F47">
         <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H47" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I47" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J47" t="s">
         <v>16</v>
@@ -2194,28 +2203,28 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F48">
         <v>40</v>
       </c>
       <c r="G48" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H48" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="I48" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="J48" t="s">
         <v>16</v>
@@ -2223,25 +2232,25 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49">
+        <v>40</v>
+      </c>
+      <c r="G49" t="s">
+        <v>101</v>
+      </c>
+      <c r="H49" t="s">
         <v>107</v>
-      </c>
-      <c r="D49">
-        <v>2</v>
-      </c>
-      <c r="E49" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49">
-        <v>50</v>
-      </c>
-      <c r="G49" t="s">
-        <v>98</v>
-      </c>
-      <c r="H49" t="s">
-        <v>104</v>
       </c>
       <c r="I49" t="s">
         <v>54</v>
@@ -2252,28 +2261,28 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="F50">
         <v>40</v>
       </c>
       <c r="G50" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H50" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="I50" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="J50" t="s">
         <v>16</v>
@@ -2281,28 +2290,28 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F51">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G51" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H51" t="s">
         <v>31</v>
       </c>
       <c r="I51" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J51" t="s">
         <v>16</v>
@@ -2310,28 +2319,28 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>110</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
-        <v>19</v>
-      </c>
       <c r="F52">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H52" t="s">
         <v>31</v>
       </c>
       <c r="I52" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J52" t="s">
         <v>16</v>
@@ -2339,28 +2348,28 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F53">
         <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H53" t="s">
         <v>31</v>
       </c>
       <c r="I53" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J53" t="s">
         <v>16</v>
@@ -2368,28 +2377,28 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F54">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H54" t="s">
         <v>31</v>
       </c>
       <c r="I54" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="J54" t="s">
         <v>16</v>
@@ -2397,28 +2406,28 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="F55">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H55" t="s">
         <v>31</v>
       </c>
       <c r="I55" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J55" t="s">
         <v>16</v>
@@ -2426,28 +2435,28 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="F56">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G56" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H56" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="I56" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="J56" t="s">
         <v>16</v>
@@ -2455,28 +2464,28 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D57">
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F57">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G57" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H57" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I57" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J57" t="s">
         <v>16</v>
@@ -2484,28 +2493,28 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="F58">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G58" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H58" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I58" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J58" t="s">
         <v>16</v>
@@ -2513,28 +2522,28 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F59">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G59" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H59" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J59" t="s">
         <v>16</v>
@@ -2542,28 +2551,28 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F60">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G60" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H60" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I60" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J60" t="s">
         <v>16</v>
@@ -2571,28 +2580,28 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="F61">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G61" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H61" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I61" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J61" t="s">
         <v>16</v>
@@ -2600,28 +2609,28 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="B62" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="F62">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G62" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H62" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I62" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="J62" t="s">
         <v>16</v>
@@ -2629,28 +2638,28 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F63">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G63" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H63" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I63" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J63" t="s">
         <v>16</v>
@@ -2658,28 +2667,28 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="F64">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G64" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H64" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I64" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J64" t="s">
         <v>16</v>
@@ -2687,28 +2696,28 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="F65">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G65" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H65" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J65" t="s">
         <v>16</v>
@@ -2716,28 +2725,31 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66">
+        <v>50</v>
+      </c>
+      <c r="G66" t="s">
+        <v>101</v>
+      </c>
+      <c r="H66" t="s">
         <v>76</v>
       </c>
-      <c r="B66" t="s">
-        <v>77</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s">
-        <v>122</v>
-      </c>
-      <c r="F66">
-        <v>50</v>
-      </c>
-      <c r="G66" t="s">
-        <v>98</v>
-      </c>
-      <c r="H66" t="s">
-        <v>72</v>
-      </c>
       <c r="I66" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="J66" t="s">
         <v>16</v>
@@ -2745,28 +2757,28 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F67">
         <v>50</v>
       </c>
       <c r="G67" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H67" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I67" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J67" t="s">
         <v>16</v>
@@ -2774,31 +2786,28 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>128</v>
+        <v>63</v>
       </c>
       <c r="F68">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G68" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H68" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I68" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J68" t="s">
         <v>16</v>
@@ -2806,28 +2815,28 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E69" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="F69">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G69" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H69" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I69" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="J69" t="s">
         <v>16</v>
@@ -2835,28 +2844,28 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F70">
         <v>40</v>
       </c>
       <c r="G70" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H70" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I70" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="J70" t="s">
         <v>16</v>
@@ -2864,28 +2873,28 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="F71">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G71" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H71" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I71" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J71" t="s">
         <v>16</v>
@@ -2893,28 +2902,28 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="F72">
         <v>80</v>
       </c>
       <c r="G72" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H72" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I72" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J72" t="s">
         <v>16</v>
@@ -2922,28 +2931,28 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
+        <v>109</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73">
+        <v>50</v>
+      </c>
+      <c r="G73" t="s">
+        <v>101</v>
+      </c>
+      <c r="H73" t="s">
         <v>90</v>
       </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73">
-        <v>40</v>
-      </c>
-      <c r="G73" t="s">
-        <v>98</v>
-      </c>
-      <c r="H73" t="s">
-        <v>88</v>
-      </c>
       <c r="I73" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J73" t="s">
         <v>16</v>
@@ -2951,28 +2960,28 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>135</v>
+      </c>
+      <c r="F74">
+        <v>50</v>
+      </c>
+      <c r="G74" t="s">
+        <v>101</v>
+      </c>
+      <c r="H74" t="s">
         <v>90</v>
       </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74">
-        <v>40</v>
-      </c>
-      <c r="G74" t="s">
-        <v>98</v>
-      </c>
-      <c r="H74" t="s">
-        <v>88</v>
-      </c>
       <c r="I74" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J74" t="s">
         <v>16</v>
@@ -2980,28 +2989,28 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="B75" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75">
+        <v>50</v>
+      </c>
+      <c r="G75" t="s">
+        <v>101</v>
+      </c>
+      <c r="H75" t="s">
         <v>90</v>
       </c>
-      <c r="D75">
-        <v>6</v>
-      </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75">
-        <v>40</v>
-      </c>
-      <c r="G75" t="s">
-        <v>98</v>
-      </c>
-      <c r="H75" t="s">
-        <v>88</v>
-      </c>
       <c r="I75" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="J75" t="s">
         <v>16</v>
@@ -3009,28 +3018,28 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="B76" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="D76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F76">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G76" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H76" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I76" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J76" t="s">
         <v>16</v>
@@ -3038,28 +3047,28 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="F77">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G77" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H77" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I77" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="J77" t="s">
         <v>16</v>
@@ -3067,28 +3076,28 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F78">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G78" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H78" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I78" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J78" t="s">
         <v>16</v>
@@ -3096,28 +3105,28 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E79" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="F79">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H79" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I79" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J79" t="s">
         <v>16</v>
@@ -3125,28 +3134,28 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F80">
         <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H80" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I80" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J80" t="s">
         <v>16</v>
@@ -3154,28 +3163,28 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81">
+        <v>40</v>
+      </c>
+      <c r="G81" t="s">
+        <v>101</v>
+      </c>
+      <c r="H81" t="s">
         <v>90</v>
       </c>
-      <c r="D81">
-        <v>3</v>
-      </c>
-      <c r="E81" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81">
-        <v>40</v>
-      </c>
-      <c r="G81" t="s">
-        <v>98</v>
-      </c>
-      <c r="H81" t="s">
-        <v>97</v>
-      </c>
       <c r="I81" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="J81" t="s">
         <v>16</v>
@@ -3183,28 +3192,28 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D82">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F82">
         <v>30</v>
       </c>
       <c r="G82" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H82" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I82" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J82" t="s">
         <v>16</v>
@@ -3212,28 +3221,28 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F83">
         <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H83" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I83" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="J83" t="s">
         <v>16</v>
@@ -3241,28 +3250,28 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F84">
         <v>50</v>
       </c>
       <c r="G84" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H84" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I84" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="J84" t="s">
         <v>16</v>
@@ -3270,105 +3279,140 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B85" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E85" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F85">
-        <v>80</v>
+        <v>40</v>
+      </c>
+      <c r="G85" t="s">
+        <v>101</v>
+      </c>
+      <c r="H85" t="s">
+        <v>100</v>
+      </c>
+      <c r="I85" t="s">
+        <v>50</v>
       </c>
       <c r="J85" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E86" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F86">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="G86" t="s">
+        <v>101</v>
+      </c>
+      <c r="H86" t="s">
+        <v>100</v>
+      </c>
+      <c r="I86" t="s">
+        <v>27</v>
       </c>
       <c r="J86" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F87">
         <v>50</v>
       </c>
       <c r="J87" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="B88" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E88" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="F88">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J88" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>141</v>
-      </c>
-      <c r="C89" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
       <c r="F89">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J89" t="s">
-        <v>138</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+      <c r="E90" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90">
+        <v>40</v>
+      </c>
+      <c r="J90" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3378,7 +3422,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3386,86 +3430,72 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
         <v>151</v>
       </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commented but still ugly code
</commit_message>
<xml_diff>
--- a/PythonScheduler/output.xlsx
+++ b/PythonScheduler/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="158">
   <si>
     <t>Course</t>
   </si>
@@ -83,258 +83,258 @@
     <t>Information Technology 227</t>
   </si>
   <si>
+    <t>CMSC 291</t>
+  </si>
+  <si>
+    <t>Continued Computer Science for Non-Majors</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Engineering 122, Engineering 122A</t>
+  </si>
+  <si>
+    <t>CMSC 201</t>
+  </si>
+  <si>
+    <t>Computer Science I</t>
+  </si>
+  <si>
+    <t>Hamilton, Eric</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>Public Policy 105</t>
+  </si>
+  <si>
+    <t>CMSC 202</t>
+  </si>
+  <si>
+    <t>Computer Science II</t>
+  </si>
+  <si>
+    <t>Dixon, Jeremy</t>
+  </si>
+  <si>
+    <t>CMSC 435/634</t>
+  </si>
+  <si>
+    <t>Computer Graphics</t>
+  </si>
+  <si>
+    <t>Olano, Marc</t>
+  </si>
+  <si>
+    <t>CMSC 476/676</t>
+  </si>
+  <si>
+    <t>Information Retrieval</t>
+  </si>
+  <si>
+    <t>Pearce, Claudia</t>
+  </si>
+  <si>
+    <t>Sherman Hall 014</t>
+  </si>
+  <si>
+    <t>CMSC 491/691</t>
+  </si>
+  <si>
+    <t>Spec Topic: Data Driven Design of Autonmous Systems</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Zhu, Ting</t>
+  </si>
+  <si>
+    <t>CMSC 203</t>
+  </si>
+  <si>
+    <t>Discrete Structures</t>
+  </si>
+  <si>
+    <t>Joeg, Prasanna</t>
+  </si>
+  <si>
+    <t>Sherman Hall 013</t>
+  </si>
+  <si>
+    <t>CMSC 313</t>
+  </si>
+  <si>
+    <t>Comp. Org. &amp; Assembly Lang.</t>
+  </si>
+  <si>
+    <t>Kartchner, Jeannette</t>
+  </si>
+  <si>
+    <t>Math &amp; Psychology 106</t>
+  </si>
+  <si>
+    <t>CMSC 331</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>Donyaee, Kash</t>
+  </si>
+  <si>
+    <t>Meyerhoff Chemistry 030</t>
+  </si>
+  <si>
+    <t>Johnson, Benjamin</t>
+  </si>
+  <si>
+    <t>Biological Sciences 120</t>
+  </si>
+  <si>
+    <t>CMSC 411cs</t>
+  </si>
+  <si>
+    <t>Computer Architecture</t>
+  </si>
+  <si>
+    <t>Sekyonda, Ivan</t>
+  </si>
+  <si>
+    <t>Interdisciplinary Life S 233</t>
+  </si>
+  <si>
+    <t>CMSC 447</t>
+  </si>
+  <si>
+    <t>Software Engineering I</t>
+  </si>
+  <si>
+    <t>Dutt, Abhijit</t>
+  </si>
+  <si>
+    <t>Sherman Hall 151</t>
+  </si>
+  <si>
+    <t>CMSC 201ss</t>
+  </si>
+  <si>
+    <t>14:30:00</t>
+  </si>
+  <si>
+    <t>Bargteil, Adam</t>
+  </si>
+  <si>
+    <t>CMSC 461</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>CMSC 684</t>
+  </si>
+  <si>
+    <t>Wireless Sensor Networks</t>
+  </si>
+  <si>
+    <t>Younis, Mohamed</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>CMSC 471</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Vafaei, Fereydoon</t>
+  </si>
+  <si>
+    <t>CMSC 691</t>
+  </si>
+  <si>
+    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Ferraro, Frank</t>
+  </si>
+  <si>
+    <t>CMSC 455</t>
+  </si>
+  <si>
+    <t>Numerical Computations</t>
+  </si>
+  <si>
+    <t>Squire, Jon</t>
+  </si>
+  <si>
+    <t>CMSC 491</t>
+  </si>
+  <si>
+    <t>Spec Topic: Data Science</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>17:30:00</t>
+  </si>
+  <si>
+    <t>Spec Topic: Malware</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Nicholas, Charles</t>
+  </si>
+  <si>
+    <t>CMSC 104</t>
+  </si>
+  <si>
+    <t>Problem Solving &amp; Prog.</t>
+  </si>
+  <si>
+    <t>CMSC 304</t>
+  </si>
+  <si>
+    <t>Social &amp; Ethical Issues in IT</t>
+  </si>
+  <si>
+    <t>CMSC 421</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>19:10:00</t>
+  </si>
+  <si>
+    <t>Tues/Thurs</t>
+  </si>
+  <si>
+    <t>CMSC 443/652</t>
+  </si>
+  <si>
+    <t>Cryptography and Data Security</t>
+  </si>
+  <si>
+    <t>Zhang, Haibin</t>
+  </si>
+  <si>
+    <t>Yesha, Yaacov</t>
+  </si>
+  <si>
     <t>CMSC 441</t>
   </si>
   <si>
-    <t>Engineering 122, Engineering 122A</t>
-  </si>
-  <si>
-    <t>CMSC 291</t>
-  </si>
-  <si>
-    <t>Continued Computer Science for Non-Majors</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>Sherman Hall 151</t>
-  </si>
-  <si>
-    <t>CMSC 201</t>
-  </si>
-  <si>
-    <t>Computer Science I</t>
-  </si>
-  <si>
-    <t>Hamilton, Eric</t>
-  </si>
-  <si>
-    <t>13:00:00</t>
-  </si>
-  <si>
-    <t>Public Policy 105</t>
-  </si>
-  <si>
-    <t>CMSC 202</t>
-  </si>
-  <si>
-    <t>Computer Science II</t>
-  </si>
-  <si>
-    <t>Dixon, Jeremy</t>
-  </si>
-  <si>
-    <t>CMSC 435/634</t>
-  </si>
-  <si>
-    <t>Computer Graphics</t>
-  </si>
-  <si>
-    <t>Olano, Marc</t>
-  </si>
-  <si>
-    <t>CMSC 476/676</t>
-  </si>
-  <si>
-    <t>Information Retrieval</t>
-  </si>
-  <si>
-    <t>Pearce, Claudia</t>
-  </si>
-  <si>
-    <t>Sherman Hall 014</t>
-  </si>
-  <si>
-    <t>CMSC 491/691</t>
-  </si>
-  <si>
-    <t>Spec Topic: Data Driven Design of Autonmous Systems</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Zhu, Ting</t>
-  </si>
-  <si>
-    <t>CMSC 203</t>
-  </si>
-  <si>
-    <t>Discrete Structures</t>
-  </si>
-  <si>
-    <t>Joeg, Prasanna</t>
-  </si>
-  <si>
-    <t>Sherman Hall 013</t>
-  </si>
-  <si>
-    <t>CMSC 313</t>
-  </si>
-  <si>
-    <t>Comp. Org. &amp; Assembly Lang.</t>
-  </si>
-  <si>
-    <t>Kartchner, Jeannette</t>
-  </si>
-  <si>
-    <t>Math &amp; Psychology 106</t>
-  </si>
-  <si>
-    <t>CMSC 331</t>
-  </si>
-  <si>
-    <t>Programming Languages</t>
-  </si>
-  <si>
-    <t>Donyaee, Kash</t>
-  </si>
-  <si>
-    <t>Meyerhoff Chemistry 030</t>
-  </si>
-  <si>
-    <t>Johnson, Benjamin</t>
-  </si>
-  <si>
-    <t>Biological Sciences 120</t>
-  </si>
-  <si>
-    <t>CMSC 411cs</t>
-  </si>
-  <si>
-    <t>Computer Architecture</t>
-  </si>
-  <si>
-    <t>Sekyonda, Ivan</t>
-  </si>
-  <si>
-    <t>Interdisciplinary Life S 233</t>
-  </si>
-  <si>
-    <t>CMSC 447</t>
-  </si>
-  <si>
-    <t>Software Engineering I</t>
-  </si>
-  <si>
-    <t>Dutt, Abhijit</t>
-  </si>
-  <si>
-    <t>CMSC 201ss</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t>Bargteil, Adam</t>
-  </si>
-  <si>
-    <t>CMSC 461</t>
-  </si>
-  <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>CMSC 684</t>
-  </si>
-  <si>
-    <t>Wireless Sensor Networks</t>
-  </si>
-  <si>
-    <t>Younis, Mohamed</t>
-  </si>
-  <si>
-    <t>16:00:00</t>
-  </si>
-  <si>
-    <t>CMSC 471</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence</t>
-  </si>
-  <si>
-    <t>Vafaei, Fereydoon</t>
-  </si>
-  <si>
-    <t>CMSC 691</t>
-  </si>
-  <si>
-    <t>Spec Topic: Graphical and Statistical Models of Learning</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Ferraro, Frank</t>
-  </si>
-  <si>
-    <t>CMSC 455</t>
-  </si>
-  <si>
-    <t>Numerical Computations</t>
-  </si>
-  <si>
-    <t>Squire, Jon</t>
-  </si>
-  <si>
-    <t>CMSC 491</t>
-  </si>
-  <si>
-    <t>Spec Topic: Data Science</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>17:30:00</t>
-  </si>
-  <si>
-    <t>Spec Topic: Malware</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Nicholas, Charles</t>
-  </si>
-  <si>
-    <t>CMSC 104</t>
-  </si>
-  <si>
-    <t>Problem Solving &amp; Prog.</t>
-  </si>
-  <si>
-    <t>CMSC 304</t>
-  </si>
-  <si>
-    <t>Social &amp; Ethical Issues in IT</t>
-  </si>
-  <si>
-    <t>CMSC 421</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>19:10:00</t>
-  </si>
-  <si>
-    <t>Tues/Thurs</t>
-  </si>
-  <si>
-    <t>CMSC 443/652</t>
-  </si>
-  <si>
-    <t>Cryptography and Data Security</t>
-  </si>
-  <si>
-    <t>Zhang, Haibin</t>
-  </si>
-  <si>
-    <t>Yesha, Yaacov</t>
-  </si>
-  <si>
     <t>Chang, Richard</t>
   </si>
   <si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t>CMSC 411cs Computer Architecture 3 Staff</t>
+  </si>
+  <si>
+    <t>CMSC 441 Algorithms 3 Marron, Christopher</t>
   </si>
   <si>
     <t>CMSC 684 Wireless Sensor Networks 2 Staff</t>
@@ -918,16 +921,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -936,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
@@ -944,28 +947,28 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
         <v>16</v>
@@ -973,28 +976,28 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F6">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
         <v>16</v>
@@ -1002,28 +1005,28 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
         <v>16</v>
@@ -1031,16 +1034,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>50</v>
@@ -1049,10 +1052,10 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -1060,16 +1063,19 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -1078,10 +1084,10 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
@@ -1089,31 +1095,28 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
@@ -1121,16 +1124,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -1139,10 +1142,10 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
@@ -1150,16 +1153,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>40</v>
@@ -1168,10 +1171,10 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
@@ -1179,13 +1182,13 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
         <v>57</v>
@@ -1197,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" t="s">
         <v>58</v>
@@ -1208,16 +1211,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F14">
         <v>40</v>
@@ -1226,10 +1229,10 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J14" t="s">
         <v>16</v>
@@ -1237,28 +1240,28 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F15">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
       </c>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
         <v>16</v>
@@ -1266,28 +1269,28 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
         <v>16</v>
@@ -1295,28 +1298,28 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="F17">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J17" t="s">
         <v>16</v>
@@ -1324,16 +1327,16 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F18">
         <v>40</v>
@@ -1342,10 +1345,10 @@
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
@@ -1353,16 +1356,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>40</v>
@@ -1371,10 +1374,10 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
@@ -1382,16 +1385,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="F20">
         <v>40</v>
@@ -1400,10 +1403,10 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J20" t="s">
         <v>16</v>
@@ -1411,16 +1414,16 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F21">
         <v>40</v>
@@ -1429,10 +1432,10 @@
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J21" t="s">
         <v>16</v>
@@ -1440,16 +1443,16 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="F22">
         <v>40</v>
@@ -1458,7 +1461,7 @@
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
@@ -1469,28 +1472,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F23">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
         <v>16</v>
@@ -1498,28 +1501,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J24" t="s">
         <v>16</v>
@@ -1527,28 +1530,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J25" t="s">
         <v>16</v>
@@ -1556,16 +1559,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F26">
         <v>50</v>
@@ -1574,10 +1580,10 @@
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s">
         <v>16</v>
@@ -1585,31 +1591,28 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F27">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J27" t="s">
         <v>16</v>
@@ -1617,16 +1620,16 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F28">
         <v>40</v>
@@ -1635,10 +1638,10 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I28" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J28" t="s">
         <v>16</v>
@@ -1646,16 +1649,19 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F29">
         <v>40</v>
@@ -1664,10 +1670,10 @@
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I29" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -1675,31 +1681,28 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F30">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I30" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="J30" t="s">
         <v>16</v>
@@ -1707,28 +1710,28 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F31">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
@@ -1736,16 +1739,19 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="F32">
         <v>50</v>
@@ -1754,10 +1760,10 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J32" t="s">
         <v>16</v>
@@ -1765,31 +1771,28 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="F33">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G33" t="s">
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J33" t="s">
         <v>16</v>
@@ -1797,16 +1800,16 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F34">
         <v>40</v>
@@ -1815,10 +1818,10 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J34" t="s">
         <v>16</v>
@@ -1826,16 +1829,16 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F35">
         <v>40</v>
@@ -1844,10 +1847,10 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I35" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J35" t="s">
         <v>16</v>
@@ -1855,16 +1858,16 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
         <v>96</v>
       </c>
-      <c r="B36" t="s">
-        <v>97</v>
-      </c>
       <c r="D36">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F36">
         <v>40</v>
@@ -1873,7 +1876,7 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I36" t="s">
         <v>58</v>
@@ -1884,16 +1887,16 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F37">
         <v>40</v>
@@ -1902,10 +1905,10 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I37" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J37" t="s">
         <v>16</v>
@@ -1913,16 +1916,16 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F38">
         <v>40</v>
@@ -1931,10 +1934,10 @@
         <v>20</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I38" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s">
         <v>16</v>
@@ -1942,28 +1945,28 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F39">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H39" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="I39" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J39" t="s">
         <v>16</v>
@@ -1971,28 +1974,28 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="F40">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J40" t="s">
         <v>16</v>
@@ -2000,28 +2003,28 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
         <v>104</v>
       </c>
       <c r="F41">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H41" t="s">
         <v>14</v>
       </c>
       <c r="I41" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J41" t="s">
         <v>16</v>
@@ -2029,28 +2032,28 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="F42">
         <v>40</v>
       </c>
       <c r="G42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J42" t="s">
         <v>16</v>
@@ -2058,28 +2061,28 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="F43">
         <v>40</v>
       </c>
       <c r="G43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H43" t="s">
         <v>14</v>
       </c>
       <c r="I43" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J43" t="s">
         <v>16</v>
@@ -2087,28 +2090,28 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="F44">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="I44" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="J44" t="s">
         <v>16</v>
@@ -2116,28 +2119,28 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F45">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H45" t="s">
         <v>107</v>
       </c>
       <c r="I45" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J45" t="s">
         <v>16</v>
@@ -2145,28 +2148,28 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F46">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H46" t="s">
         <v>107</v>
       </c>
       <c r="I46" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J46" t="s">
         <v>16</v>
@@ -2174,28 +2177,28 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="F47">
         <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H47" t="s">
         <v>107</v>
       </c>
       <c r="I47" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J47" t="s">
         <v>16</v>
@@ -2203,28 +2206,28 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="F48">
         <v>40</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H48" t="s">
         <v>107</v>
       </c>
       <c r="I48" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J48" t="s">
         <v>16</v>
@@ -2232,28 +2235,28 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="F49">
         <v>40</v>
       </c>
       <c r="G49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H49" t="s">
         <v>107</v>
       </c>
       <c r="I49" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J49" t="s">
         <v>16</v>
@@ -2261,28 +2264,28 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F50">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H50" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="I50" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="J50" t="s">
         <v>16</v>
@@ -2290,28 +2293,28 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F51">
         <v>50</v>
       </c>
       <c r="G51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I51" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J51" t="s">
         <v>16</v>
@@ -2319,28 +2322,28 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F52">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I52" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="J52" t="s">
         <v>16</v>
@@ -2348,28 +2351,28 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="F53">
         <v>40</v>
       </c>
       <c r="G53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I53" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J53" t="s">
         <v>16</v>
@@ -2377,28 +2380,28 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="F54">
         <v>40</v>
       </c>
       <c r="G54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H54" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I54" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J54" t="s">
         <v>16</v>
@@ -2406,28 +2409,28 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>11</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="F55">
         <v>40</v>
       </c>
       <c r="G55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I55" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J55" t="s">
         <v>16</v>
@@ -2435,28 +2438,28 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="F56">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H56" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="I56" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="J56" t="s">
         <v>16</v>
@@ -2464,28 +2467,28 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="F57">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J57" t="s">
         <v>16</v>
@@ -2493,28 +2496,28 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F58">
         <v>50</v>
       </c>
       <c r="G58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I58" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J58" t="s">
         <v>16</v>
@@ -2522,28 +2525,28 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F59">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I59" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J59" t="s">
         <v>16</v>
@@ -2551,28 +2554,28 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="F60">
         <v>40</v>
       </c>
       <c r="G60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I60" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="J60" t="s">
         <v>16</v>
@@ -2580,28 +2583,28 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="F61">
         <v>40</v>
       </c>
       <c r="G61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I61" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="J61" t="s">
         <v>16</v>
@@ -2609,28 +2612,28 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="F62">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H62" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I62" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="J62" t="s">
         <v>16</v>
@@ -2638,28 +2641,28 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="F63">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I63" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J63" t="s">
         <v>16</v>
@@ -2667,28 +2670,28 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F64">
         <v>50</v>
       </c>
       <c r="G64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I64" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J64" t="s">
         <v>16</v>
@@ -2696,28 +2699,31 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>43</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F65">
         <v>50</v>
       </c>
       <c r="G65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I65" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="J65" t="s">
         <v>16</v>
@@ -2725,31 +2731,28 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F66">
         <v>50</v>
       </c>
       <c r="G66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I66" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="J66" t="s">
         <v>16</v>
@@ -2757,28 +2760,28 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="F67">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I67" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="J67" t="s">
         <v>16</v>
@@ -2786,28 +2789,28 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B68" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68" t="s">
+        <v>78</v>
+      </c>
+      <c r="F68">
+        <v>40</v>
+      </c>
+      <c r="G68" t="s">
+        <v>100</v>
+      </c>
+      <c r="H68" t="s">
+        <v>75</v>
+      </c>
+      <c r="I68" t="s">
         <v>52</v>
-      </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s">
-        <v>63</v>
-      </c>
-      <c r="F68">
-        <v>40</v>
-      </c>
-      <c r="G68" t="s">
-        <v>101</v>
-      </c>
-      <c r="H68" t="s">
-        <v>76</v>
-      </c>
-      <c r="I68" t="s">
-        <v>50</v>
       </c>
       <c r="J68" t="s">
         <v>16</v>
@@ -2815,28 +2818,28 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="D69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F69">
         <v>40</v>
       </c>
       <c r="G69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I69" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J69" t="s">
         <v>16</v>
@@ -2844,28 +2847,28 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="F70">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H70" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I70" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="J70" t="s">
         <v>16</v>
@@ -2873,28 +2876,28 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="F71">
         <v>80</v>
       </c>
       <c r="G71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H71" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I71" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="J71" t="s">
         <v>16</v>
@@ -2902,28 +2905,28 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F72">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I72" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="J72" t="s">
         <v>16</v>
@@ -2931,28 +2934,28 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="F73">
         <v>50</v>
       </c>
       <c r="G73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I73" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="J73" t="s">
         <v>16</v>
@@ -2960,28 +2963,28 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="F74">
         <v>50</v>
       </c>
       <c r="G74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I74" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="J74" t="s">
         <v>16</v>
@@ -2989,28 +2992,28 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F75">
         <v>50</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I75" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="J75" t="s">
         <v>16</v>
@@ -3024,22 +3027,22 @@
         <v>137</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="F76">
         <v>50</v>
       </c>
       <c r="G76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I76" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="J76" t="s">
         <v>16</v>
@@ -3047,28 +3050,28 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="F77">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I77" t="s">
-        <v>138</v>
+        <v>48</v>
       </c>
       <c r="J77" t="s">
         <v>16</v>
@@ -3076,28 +3079,28 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" t="s">
         <v>94</v>
       </c>
-      <c r="B78" t="s">
-        <v>95</v>
-      </c>
       <c r="D78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E78" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F78">
         <v>40</v>
       </c>
       <c r="G78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I78" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J78" t="s">
         <v>16</v>
@@ -3105,28 +3108,28 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F79">
         <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I79" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J79" t="s">
         <v>16</v>
@@ -3134,28 +3137,28 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" t="s">
         <v>96</v>
       </c>
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
       <c r="D80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F80">
         <v>40</v>
       </c>
       <c r="G80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I80" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J80" t="s">
         <v>16</v>
@@ -3163,28 +3166,28 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F81">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I81" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J81" t="s">
         <v>16</v>
@@ -3192,28 +3195,28 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="F82">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G82" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H82" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I82" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J82" t="s">
         <v>16</v>
@@ -3221,28 +3224,28 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F83">
         <v>50</v>
       </c>
       <c r="G83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H83" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I83" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J83" t="s">
         <v>16</v>
@@ -3250,28 +3253,28 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E84" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="F84">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I84" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="J84" t="s">
         <v>16</v>
@@ -3279,28 +3282,28 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E85" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F85">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H85" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I85" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J85" t="s">
         <v>16</v>
@@ -3308,48 +3311,39 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D86">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F86">
-        <v>30</v>
-      </c>
-      <c r="G86" t="s">
-        <v>101</v>
-      </c>
-      <c r="H86" t="s">
-        <v>100</v>
-      </c>
-      <c r="I86" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="J86" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B87" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E87" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F87">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J87" t="s">
         <v>144</v>
@@ -3357,16 +3351,16 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="D88">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E88" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F88">
         <v>40</v>
@@ -3377,16 +3371,16 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B89" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D89">
         <v>3</v>
       </c>
       <c r="E89" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F89">
         <v>40</v>
@@ -3397,16 +3391,16 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" t="s">
         <v>73</v>
-      </c>
-      <c r="B90" t="s">
-        <v>74</v>
       </c>
       <c r="D90">
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F90">
         <v>40</v>
@@ -3422,7 +3416,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3498,6 +3492,20 @@
         <v>154</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>